<commit_message>
Added Raid Calculation Section
</commit_message>
<xml_diff>
--- a/Dragalia Data.xlsx
+++ b/Dragalia Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aff98139d4bac41f/文件/DL/dragalia-data-track/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="14_{049F9EFC-050E-4651-8DC8-B33E922A69AE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{129F0FAD-B3FA-4EFA-960D-3CD7177B9971}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="14_{049F9EFC-050E-4651-8DC8-B33E922A69AE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{833477C4-E9A8-40CD-BA5A-EFC712428BE4}"/>
   <bookViews>
-    <workbookView xWindow="-22905" yWindow="2580" windowWidth="20850" windowHeight="11820" activeTab="1" xr2:uid="{D0E79A60-AC9E-4AFD-A74C-CCE50AE0356B}"/>
+    <workbookView xWindow="1860" yWindow="1770" windowWidth="20850" windowHeight="11820" activeTab="6" xr2:uid="{D0E79A60-AC9E-4AFD-A74C-CCE50AE0356B}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="112">
   <si>
     <t>STR %</t>
   </si>
@@ -924,7 +924,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="239">
+  <cellXfs count="248">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1388,6 +1388,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1454,39 +1505,39 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="169" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1575,18 +1626,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1626,18 +1665,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1970,8 +1997,8 @@
   </sheetPr>
   <dimension ref="A1:AJ40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="V37" sqref="V37"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="X34" sqref="X34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2001,46 +2028,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="201" t="s">
+      <c r="A1" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
-      <c r="L1" s="201"/>
-      <c r="M1" s="201"/>
-      <c r="N1" s="201"/>
-      <c r="O1" s="201"/>
-      <c r="P1" s="201"/>
-      <c r="Q1" s="202"/>
+      <c r="B1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="218"/>
+      <c r="I1" s="218"/>
+      <c r="J1" s="218"/>
+      <c r="K1" s="218"/>
+      <c r="L1" s="218"/>
+      <c r="M1" s="218"/>
+      <c r="N1" s="218"/>
+      <c r="O1" s="218"/>
+      <c r="P1" s="218"/>
+      <c r="Q1" s="219"/>
       <c r="R1" s="76"/>
-      <c r="S1" s="201" t="s">
+      <c r="S1" s="218" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="201"/>
-      <c r="U1" s="201"/>
-      <c r="V1" s="201"/>
-      <c r="W1" s="201"/>
-      <c r="X1" s="201"/>
-      <c r="Y1" s="201"/>
-      <c r="Z1" s="201"/>
-      <c r="AA1" s="201"/>
-      <c r="AB1" s="201"/>
-      <c r="AC1" s="201"/>
-      <c r="AD1" s="201"/>
-      <c r="AE1" s="201"/>
-      <c r="AF1" s="201"/>
-      <c r="AG1" s="201"/>
-      <c r="AH1" s="201"/>
-      <c r="AI1" s="201"/>
-      <c r="AJ1" s="202"/>
+      <c r="T1" s="218"/>
+      <c r="U1" s="218"/>
+      <c r="V1" s="218"/>
+      <c r="W1" s="218"/>
+      <c r="X1" s="218"/>
+      <c r="Y1" s="218"/>
+      <c r="Z1" s="218"/>
+      <c r="AA1" s="218"/>
+      <c r="AB1" s="218"/>
+      <c r="AC1" s="218"/>
+      <c r="AD1" s="218"/>
+      <c r="AE1" s="218"/>
+      <c r="AF1" s="218"/>
+      <c r="AG1" s="218"/>
+      <c r="AH1" s="218"/>
+      <c r="AI1" s="218"/>
+      <c r="AJ1" s="219"/>
     </row>
     <row r="2" spans="1:36" s="127" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="127" t="s">
@@ -2061,13 +2088,13 @@
       <c r="G2" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="217" t="s">
+      <c r="H2" s="234" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="217"/>
-      <c r="J2" s="217"/>
-      <c r="K2" s="217"/>
-      <c r="L2" s="217"/>
+      <c r="I2" s="234"/>
+      <c r="J2" s="234"/>
+      <c r="K2" s="234"/>
+      <c r="L2" s="234"/>
       <c r="M2" s="127" t="s">
         <v>38</v>
       </c>
@@ -2084,50 +2111,50 @@
         <v>42</v>
       </c>
       <c r="S2" s="139"/>
-      <c r="T2" s="184" t="s">
+      <c r="T2" s="200" t="s">
         <v>38</v>
       </c>
-      <c r="U2" s="184" t="s">
+      <c r="U2" s="200" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="184" t="s">
+      <c r="V2" s="200" t="s">
         <v>46</v>
       </c>
-      <c r="W2" s="184" t="s">
+      <c r="W2" s="200" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="184" t="s">
+      <c r="X2" s="200" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="184" t="s">
+      <c r="Y2" s="200" t="s">
         <v>41</v>
       </c>
-      <c r="Z2" s="184"/>
-      <c r="AA2" s="193" t="s">
+      <c r="Z2" s="200"/>
+      <c r="AA2" s="210" t="s">
         <v>50</v>
       </c>
-      <c r="AB2" s="184"/>
-      <c r="AC2" s="184"/>
-      <c r="AD2" s="184"/>
-      <c r="AE2" s="184"/>
-      <c r="AF2" s="184" t="s">
+      <c r="AB2" s="200"/>
+      <c r="AC2" s="200"/>
+      <c r="AD2" s="200"/>
+      <c r="AE2" s="200"/>
+      <c r="AF2" s="200" t="s">
         <v>51</v>
       </c>
-      <c r="AG2" s="184"/>
-      <c r="AH2" s="184"/>
-      <c r="AI2" s="184"/>
-      <c r="AJ2" s="194"/>
+      <c r="AG2" s="200"/>
+      <c r="AH2" s="200"/>
+      <c r="AI2" s="200"/>
+      <c r="AJ2" s="211"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="142">
-        <v>2983</v>
+        <v>2883</v>
       </c>
       <c r="C3" s="61">
         <f>SUM(I11:I12,R11:R12)</f>
-        <v>2620</v>
+        <v>2520</v>
       </c>
       <c r="D3" s="61">
         <f>E3-G3</f>
@@ -2145,14 +2172,14 @@
         <f>IF(C3-B3 &lt; 0, 0, C3-B3)</f>
         <v>0</v>
       </c>
-      <c r="H3" s="197">
+      <c r="H3" s="214">
         <f t="shared" ref="H3:H8" si="0">IF(D3/E3 &gt; 1, 100%, D3/E3)</f>
         <v>1</v>
       </c>
-      <c r="I3" s="197"/>
-      <c r="J3" s="197"/>
-      <c r="K3" s="197"/>
-      <c r="L3" s="197"/>
+      <c r="I3" s="214"/>
+      <c r="J3" s="214"/>
+      <c r="K3" s="214"/>
+      <c r="L3" s="214"/>
       <c r="M3" s="18">
         <f>IFERROR(ROUND(G3/P3, 0),"")</f>
         <v>0</v>
@@ -2175,13 +2202,13 @@
       </c>
       <c r="R3" s="18"/>
       <c r="S3" s="139"/>
-      <c r="T3" s="184"/>
-      <c r="U3" s="184"/>
-      <c r="V3" s="184"/>
-      <c r="W3" s="184"/>
-      <c r="X3" s="184"/>
-      <c r="Y3" s="184"/>
-      <c r="Z3" s="184"/>
+      <c r="T3" s="200"/>
+      <c r="U3" s="200"/>
+      <c r="V3" s="200"/>
+      <c r="W3" s="200"/>
+      <c r="X3" s="200"/>
+      <c r="Y3" s="200"/>
+      <c r="Z3" s="200"/>
       <c r="AA3" s="137">
         <v>2</v>
       </c>
@@ -2218,11 +2245,11 @@
         <v>12</v>
       </c>
       <c r="B4" s="142">
-        <v>1984</v>
+        <v>1708</v>
       </c>
       <c r="C4" s="61">
         <f>SUM(I13:I14,R13:R14)</f>
-        <v>1560</v>
+        <v>1360</v>
       </c>
       <c r="D4" s="61">
         <f>E4-G4</f>
@@ -2234,20 +2261,20 @@
       </c>
       <c r="F4" s="142">
         <f>IF(C4-B4 &lt; 0, ABS(C4-B4), "")</f>
-        <v>424</v>
+        <v>348</v>
       </c>
       <c r="G4" s="5">
         <f>IF(C4-B4 &lt; 0, 0, C4-B4)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="197">
+      <c r="H4" s="214">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I4" s="197"/>
-      <c r="J4" s="197"/>
-      <c r="K4" s="197"/>
-      <c r="L4" s="197"/>
+      <c r="I4" s="214"/>
+      <c r="J4" s="214"/>
+      <c r="K4" s="214"/>
+      <c r="L4" s="214"/>
       <c r="M4" s="17">
         <f>IFERROR(ROUND(G4/P4, 0),"")</f>
         <v>0</v>
@@ -2262,80 +2289,79 @@
       </c>
       <c r="P4" s="22">
         <f>IFERROR((SUM(_DataIO!D:D) * 3 + SUM(_DataIO!E:E) * 4) / Q4, "")</f>
-        <v>3.4834123222748814</v>
+        <v>3.4778660612939842</v>
       </c>
       <c r="Q4" s="92">
         <f>SUM(_DataIO!D:E)</f>
-        <v>844</v>
+        <v>881</v>
       </c>
       <c r="R4" s="17"/>
-      <c r="S4" s="199" t="s">
+      <c r="S4" s="216" t="s">
         <v>43</v>
       </c>
-      <c r="T4" s="181">
+      <c r="T4" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, COUNTA(DATA_HDRAG_HBRUN), "")</f>
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="U4" s="130">
         <f>IF(HDRAG_HAS_REC_HBRUN, COUNTIF(DATA_HDRAG_HBRUN, "=2"), "")</f>
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="V4" s="130">
         <f>IF(HDRAG_HAS_REC_HBRUN, COUNTIF(DATA_HDRAG_HBRUN, "=3"), "")</f>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="W4" s="130">
         <f>IF(HDRAG_HAS_REC_HBRUN, COUNTIF(DATA_HDRAG_HBRUN, "=4"), "")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="X4" s="130">
-        <f>IF(HDRAG_HAS_REC_HBRUN, COUNTIF(DATA_HDRAG_HBRUN, "=5"), "")</f>
         <v>4</v>
       </c>
-      <c r="Y4" s="196">
+      <c r="Y4" s="213">
         <f>IF(HDRAG_HAS_REC_HBRUN,AVERAGE(DATA_HDRAG_HBRUN),"")</f>
-        <v>2.4210526315789473</v>
-      </c>
-      <c r="Z4" s="196"/>
-      <c r="AA4" s="192">
+        <v>2.3986928104575163</v>
+      </c>
+      <c r="Z4" s="213"/>
+      <c r="AA4" s="209">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y4)*U5), "")</f>
-        <v>139</v>
-      </c>
-      <c r="AB4" s="181">
+        <v>143</v>
+      </c>
+      <c r="AB4" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y4)*V5), "")</f>
-        <v>46</v>
-      </c>
-      <c r="AC4" s="181">
+        <v>44</v>
+      </c>
+      <c r="AC4" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y4)*W5), "")</f>
         <v>11</v>
       </c>
-      <c r="AD4" s="181">
+      <c r="AD4" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y4)*X5), "")</f>
-        <v>7</v>
-      </c>
-      <c r="AE4" s="195">
+        <v>6</v>
+      </c>
+      <c r="AE4" s="212">
         <f>IF(HDRAG_HAS_REC_HBRUN, SUM(AA4:AD4), "")</f>
-        <v>203</v>
-      </c>
-      <c r="AF4" s="181">
+        <v>204</v>
+      </c>
+      <c r="AF4" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y4)*U5), "")</f>
-        <v>234</v>
-      </c>
-      <c r="AG4" s="181">
+        <v>241</v>
+      </c>
+      <c r="AG4" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y4)*V5), "")</f>
-        <v>77</v>
-      </c>
-      <c r="AH4" s="181">
+        <v>74</v>
+      </c>
+      <c r="AH4" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y4)*W5), "")</f>
         <v>18</v>
       </c>
-      <c r="AI4" s="181">
+      <c r="AI4" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y4)*X5), "")</f>
-        <v>11</v>
-      </c>
-      <c r="AJ4" s="185">
+        <v>9</v>
+      </c>
+      <c r="AJ4" s="201">
         <f>IF(HDRAG_HAS_REC_HBRUN, SUM(AF4:AI4), "")</f>
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2343,7 +2369,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="142">
-        <v>385</v>
+        <v>521</v>
       </c>
       <c r="C5" s="61">
         <f>SUM(I15:I16,R15:R16)</f>
@@ -2359,20 +2385,20 @@
       </c>
       <c r="F5" s="142">
         <f>IF(C5-B5 &lt; 0, ABS(C5-B5), "")</f>
-        <v>225</v>
+        <v>361</v>
       </c>
       <c r="G5" s="5">
         <f>IF(C5-B5 &lt; 0, 0, C5-B5)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="197">
+      <c r="H5" s="214">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I5" s="197"/>
-      <c r="J5" s="197"/>
-      <c r="K5" s="197"/>
-      <c r="L5" s="197"/>
+      <c r="I5" s="214"/>
+      <c r="J5" s="214"/>
+      <c r="K5" s="214"/>
+      <c r="L5" s="214"/>
       <c r="M5" s="19">
         <f>IFERROR(ROUND(G5/P5, 0),"")</f>
         <v>0</v>
@@ -2387,50 +2413,50 @@
       </c>
       <c r="P5" s="23">
         <f>IFERROR((SUM(_DataIO!G:G) * 3 + SUM(_DataIO!H:H) * 4) / Q5, "")</f>
-        <v>3.4893617021276597</v>
+        <v>3.492957746478873</v>
       </c>
       <c r="Q5" s="93">
         <f>SUM(_DataIO!G:H)</f>
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="R5" s="19"/>
-      <c r="S5" s="199"/>
-      <c r="T5" s="181"/>
+      <c r="S5" s="216"/>
+      <c r="T5" s="197"/>
       <c r="U5" s="86">
         <f>IF(HDRAG_HAS_REC_HBRUN, U4/$T4, "")</f>
-        <v>0.69172932330827064</v>
+        <v>0.70588235294117652</v>
       </c>
       <c r="V5" s="86">
         <f>IF(HDRAG_HAS_REC_HBRUN, V4/$T4, "")</f>
-        <v>0.22556390977443608</v>
+        <v>0.21568627450980393</v>
       </c>
       <c r="W5" s="86">
         <f>IF(HDRAG_HAS_REC_HBRUN, W4/$T4, "")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>5.2287581699346407E-2</v>
       </c>
       <c r="X5" s="86">
         <f>IF(HDRAG_HAS_REC_HBRUN, X4/$T4, "")</f>
-        <v>3.007518796992481E-2</v>
-      </c>
-      <c r="Y5" s="196"/>
-      <c r="Z5" s="196"/>
-      <c r="AA5" s="192"/>
-      <c r="AB5" s="181"/>
-      <c r="AC5" s="181"/>
-      <c r="AD5" s="181"/>
-      <c r="AE5" s="195"/>
-      <c r="AF5" s="181"/>
-      <c r="AG5" s="181"/>
-      <c r="AH5" s="181"/>
-      <c r="AI5" s="181"/>
-      <c r="AJ5" s="185"/>
+        <v>2.6143790849673203E-2</v>
+      </c>
+      <c r="Y5" s="213"/>
+      <c r="Z5" s="213"/>
+      <c r="AA5" s="209"/>
+      <c r="AB5" s="197"/>
+      <c r="AC5" s="197"/>
+      <c r="AD5" s="197"/>
+      <c r="AE5" s="212"/>
+      <c r="AF5" s="197"/>
+      <c r="AG5" s="197"/>
+      <c r="AH5" s="197"/>
+      <c r="AI5" s="197"/>
+      <c r="AJ5" s="201"/>
     </row>
     <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="142">
-        <v>394</v>
+        <v>418</v>
       </c>
       <c r="C6" s="61">
         <f>SUM(I17:I18)</f>
@@ -2446,20 +2472,20 @@
       </c>
       <c r="F6" s="142">
         <f>IF(C6-B6 &lt; 0, ABS(C6-B6), "")</f>
-        <v>394</v>
+        <v>418</v>
       </c>
       <c r="G6" s="5">
         <f>IF(C6-B6 &lt; 0, 0, C6-B6)</f>
         <v>0</v>
       </c>
-      <c r="H6" s="197">
+      <c r="H6" s="214">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I6" s="197"/>
-      <c r="J6" s="197"/>
-      <c r="K6" s="197"/>
-      <c r="L6" s="197"/>
+      <c r="I6" s="214"/>
+      <c r="J6" s="214"/>
+      <c r="K6" s="214"/>
+      <c r="L6" s="214"/>
       <c r="M6" s="20">
         <f>IFERROR(ROUND(G6/P6, 0),"")</f>
         <v>0</v>
@@ -2474,17 +2500,17 @@
       </c>
       <c r="P6" s="24">
         <f>IFERROR((SUM(_DataIO!J:J) * 3 + SUM(_DataIO!K:K) * 4) / Q6, "")</f>
-        <v>3.5027777777777778</v>
+        <v>3.5145888594164458</v>
       </c>
       <c r="Q6" s="94">
         <f>SUM(_DataIO!J:K)</f>
-        <v>360</v>
+        <v>377</v>
       </c>
       <c r="R6" s="20"/>
-      <c r="S6" s="200" t="s">
+      <c r="S6" s="217" t="s">
         <v>57</v>
       </c>
-      <c r="T6" s="176" t="str">
+      <c r="T6" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, COUNTA(DATA_HDRAG_HMERC), "")</f>
         <v/>
       </c>
@@ -2504,48 +2530,48 @@
         <f>IF(HDRAG_HAS_REC_HMERC, COUNTIF(DATA_HDRAG_HMERC, "=5"), "")</f>
         <v/>
       </c>
-      <c r="Y6" s="188" t="str">
+      <c r="Y6" s="205" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC,AVERAGE(DATA_HDRAG_HMERC),"")</f>
         <v/>
       </c>
-      <c r="Z6" s="188"/>
-      <c r="AA6" s="187" t="str">
+      <c r="Z6" s="205"/>
+      <c r="AA6" s="203" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y6)*U7), "")</f>
         <v/>
       </c>
-      <c r="AB6" s="176" t="str">
+      <c r="AB6" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y6)*V7), "")</f>
         <v/>
       </c>
-      <c r="AC6" s="176" t="str">
+      <c r="AC6" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y6)*W7), "")</f>
         <v/>
       </c>
-      <c r="AD6" s="176" t="str">
+      <c r="AD6" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y6)*X7), "")</f>
         <v/>
       </c>
-      <c r="AE6" s="177" t="str">
+      <c r="AE6" s="204" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, SUM(AA6:AD6), "")</f>
         <v/>
       </c>
-      <c r="AF6" s="176" t="str">
+      <c r="AF6" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y6)*U7), "")</f>
         <v/>
       </c>
-      <c r="AG6" s="176" t="str">
+      <c r="AG6" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y6)*V7), "")</f>
         <v/>
       </c>
-      <c r="AH6" s="176" t="str">
+      <c r="AH6" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y6)*W7), "")</f>
         <v/>
       </c>
-      <c r="AI6" s="176" t="str">
+      <c r="AI6" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y6)*X7), "")</f>
         <v/>
       </c>
-      <c r="AJ6" s="186" t="str">
+      <c r="AJ6" s="202" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, SUM(AF6:AI6), "")</f>
         <v/>
       </c>
@@ -2555,7 +2581,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="142">
-        <v>510</v>
+        <v>711</v>
       </c>
       <c r="C7" s="61">
         <f>SUM(R17:R18)</f>
@@ -2571,20 +2597,20 @@
       </c>
       <c r="F7" s="142">
         <f>IF(C7-B7 &lt; 0, ABS(C7-B7), "")</f>
-        <v>510</v>
+        <v>711</v>
       </c>
       <c r="G7" s="5">
         <f>IF(C7-B7 &lt; 0, 0, C7-B7)</f>
         <v>0</v>
       </c>
-      <c r="H7" s="197">
+      <c r="H7" s="214">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I7" s="197"/>
-      <c r="J7" s="197"/>
-      <c r="K7" s="197"/>
-      <c r="L7" s="197"/>
+      <c r="I7" s="214"/>
+      <c r="J7" s="214"/>
+      <c r="K7" s="214"/>
+      <c r="L7" s="214"/>
       <c r="M7" s="16">
         <f>IFERROR(ROUND(G7/P7, 0),"")</f>
         <v>0</v>
@@ -2606,8 +2632,8 @@
         <v>229</v>
       </c>
       <c r="R7" s="16"/>
-      <c r="S7" s="200"/>
-      <c r="T7" s="176"/>
+      <c r="S7" s="217"/>
+      <c r="T7" s="193"/>
       <c r="U7" s="87" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, U6/$T6, "")</f>
         <v/>
@@ -2624,18 +2650,18 @@
         <f>IF(HDRAG_HAS_REC_HMERC, X6/$T6, "")</f>
         <v/>
       </c>
-      <c r="Y7" s="188"/>
-      <c r="Z7" s="188"/>
-      <c r="AA7" s="187"/>
-      <c r="AB7" s="176"/>
-      <c r="AC7" s="176"/>
-      <c r="AD7" s="176"/>
-      <c r="AE7" s="177"/>
-      <c r="AF7" s="176"/>
-      <c r="AG7" s="176"/>
-      <c r="AH7" s="176"/>
-      <c r="AI7" s="176"/>
-      <c r="AJ7" s="186"/>
+      <c r="Y7" s="205"/>
+      <c r="Z7" s="205"/>
+      <c r="AA7" s="203"/>
+      <c r="AB7" s="193"/>
+      <c r="AC7" s="193"/>
+      <c r="AD7" s="193"/>
+      <c r="AE7" s="204"/>
+      <c r="AF7" s="193"/>
+      <c r="AG7" s="193"/>
+      <c r="AH7" s="193"/>
+      <c r="AI7" s="193"/>
+      <c r="AJ7" s="202"/>
     </row>
     <row r="8" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -2643,11 +2669,11 @@
       </c>
       <c r="B8" s="142">
         <f t="shared" ref="B8:G8" si="1">SUM(B3:B7)</f>
-        <v>6256</v>
+        <v>6241</v>
       </c>
       <c r="C8" s="61">
         <f t="shared" si="1"/>
-        <v>4340</v>
+        <v>4040</v>
       </c>
       <c r="D8" s="61">
         <f t="shared" si="1"/>
@@ -2659,20 +2685,20 @@
       </c>
       <c r="F8" s="142">
         <f t="shared" si="1"/>
-        <v>1916</v>
+        <v>2201</v>
       </c>
       <c r="G8" s="142">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H8" s="197">
+      <c r="H8" s="214">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I8" s="197"/>
-      <c r="J8" s="197"/>
-      <c r="K8" s="197"/>
-      <c r="L8" s="197"/>
+      <c r="I8" s="214"/>
+      <c r="J8" s="214"/>
+      <c r="K8" s="214"/>
+      <c r="L8" s="214"/>
       <c r="M8" s="3">
         <f>SUM(M3:M7)</f>
         <v>0</v>
@@ -2687,17 +2713,17 @@
       </c>
       <c r="P8" s="26">
         <f>(SUM(_DataIO!A:A, _DataIO!D:D, _DataIO!G:G, _DataIO!J:J, _DataIO!M:M) * 3 + SUM(_DataIO!B:B, _DataIO!E:E, _DataIO!H:H, _DataIO!K:K, _DataIO!N:N) * 4) / Q8</f>
-        <v>3.5135692201992441</v>
+        <v>3.5131490222521915</v>
       </c>
       <c r="Q8" s="96">
         <f>SUM(Q3:Q7)</f>
-        <v>2911</v>
+        <v>2966</v>
       </c>
       <c r="R8" s="3"/>
-      <c r="S8" s="189" t="s">
+      <c r="S8" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="T8" s="162">
+      <c r="T8" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, COUNTA(DATA_HDRAG_HMID), "")</f>
         <v>798</v>
       </c>
@@ -2717,56 +2743,56 @@
         <f>IF(HDRAG_HAS_REC_HMID, COUNTIF(DATA_HDRAG_HMID, "=5"), "")</f>
         <v>49</v>
       </c>
-      <c r="Y8" s="164">
+      <c r="Y8" s="181">
         <f>IF(HDRAG_HAS_REC_HMID,AVERAGE(DATA_HDRAG_HMID),"")</f>
         <v>2.5513784461152884</v>
       </c>
-      <c r="Z8" s="164"/>
-      <c r="AA8" s="171">
+      <c r="Z8" s="181"/>
+      <c r="AA8" s="188">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y8)*U9), "")</f>
         <v>124</v>
       </c>
-      <c r="AB8" s="162">
+      <c r="AB8" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y8)*V9), "")</f>
         <v>41</v>
       </c>
-      <c r="AC8" s="162">
+      <c r="AC8" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y8)*W9), "")</f>
         <v>15</v>
       </c>
-      <c r="AD8" s="162">
+      <c r="AD8" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y8)*X9), "")</f>
         <v>12</v>
       </c>
-      <c r="AE8" s="161">
+      <c r="AE8" s="178">
         <f>IF(HDRAG_HAS_REC_HMID, SUM(AA8:AD8), "")</f>
         <v>192</v>
       </c>
-      <c r="AF8" s="162">
+      <c r="AF8" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y8)*U9), "")</f>
         <v>208</v>
       </c>
-      <c r="AG8" s="162">
+      <c r="AG8" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y8)*V9), "")</f>
         <v>68</v>
       </c>
-      <c r="AH8" s="162">
+      <c r="AH8" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y8)*W9), "")</f>
         <v>25</v>
       </c>
-      <c r="AI8" s="162">
+      <c r="AI8" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y8)*X9), "")</f>
         <v>20</v>
       </c>
-      <c r="AJ8" s="179">
+      <c r="AJ8" s="195">
         <f>IF(HDRAG_HAS_REC_HMID, SUM(AF8:AI8), "")</f>
         <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q9" s="97"/>
-      <c r="S9" s="189"/>
-      <c r="T9" s="162"/>
+      <c r="S9" s="206"/>
+      <c r="T9" s="179"/>
       <c r="U9" s="88">
         <f>IF(HDRAG_HAS_REC_HMID, U8/$T8, "")</f>
         <v>0.64912280701754388</v>
@@ -2783,31 +2809,31 @@
         <f>IF(HDRAG_HAS_REC_HMID, X8/$T8, "")</f>
         <v>6.1403508771929821E-2</v>
       </c>
-      <c r="Y9" s="164"/>
-      <c r="Z9" s="164"/>
-      <c r="AA9" s="171"/>
-      <c r="AB9" s="162"/>
-      <c r="AC9" s="162"/>
-      <c r="AD9" s="162"/>
-      <c r="AE9" s="161"/>
-      <c r="AF9" s="162"/>
-      <c r="AG9" s="162"/>
-      <c r="AH9" s="162"/>
-      <c r="AI9" s="162"/>
-      <c r="AJ9" s="179"/>
+      <c r="Y9" s="181"/>
+      <c r="Z9" s="181"/>
+      <c r="AA9" s="188"/>
+      <c r="AB9" s="179"/>
+      <c r="AC9" s="179"/>
+      <c r="AD9" s="179"/>
+      <c r="AE9" s="178"/>
+      <c r="AF9" s="179"/>
+      <c r="AG9" s="179"/>
+      <c r="AH9" s="179"/>
+      <c r="AI9" s="179"/>
+      <c r="AJ9" s="195"/>
     </row>
     <row r="10" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="208" t="s">
+      <c r="A10" s="225" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="208"/>
+      <c r="B10" s="225"/>
       <c r="F10" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="190" t="s">
+      <c r="G10" s="207" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="191"/>
+      <c r="H10" s="208"/>
       <c r="I10" s="29"/>
       <c r="J10" s="35" t="s">
         <v>28</v>
@@ -2821,10 +2847,10 @@
       <c r="M10" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="190" t="s">
+      <c r="N10" s="207" t="s">
         <v>26</v>
       </c>
-      <c r="O10" s="191"/>
+      <c r="O10" s="208"/>
       <c r="P10" s="35" t="s">
         <v>28</v>
       </c>
@@ -2832,10 +2858,10 @@
         <v>29</v>
       </c>
       <c r="R10" s="29"/>
-      <c r="S10" s="159" t="s">
+      <c r="S10" s="176" t="s">
         <v>58</v>
       </c>
-      <c r="T10" s="160" t="str">
+      <c r="T10" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, COUNTA(DATA_HDRAG_HJUP), "")</f>
         <v/>
       </c>
@@ -2855,57 +2881,57 @@
         <f>IF(HDRAG_HAS_REC_HJUP, COUNTIF(DATA_HDRAG_HJUP, "=5"), "")</f>
         <v/>
       </c>
-      <c r="Y10" s="165" t="str">
+      <c r="Y10" s="182" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP,AVERAGE(DATA_HDRAG_HJUP),"")</f>
         <v/>
       </c>
-      <c r="Z10" s="165"/>
-      <c r="AA10" s="180" t="str">
+      <c r="Z10" s="182"/>
+      <c r="AA10" s="196" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y10)*U11), "")</f>
         <v/>
       </c>
-      <c r="AB10" s="160" t="str">
+      <c r="AB10" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y10)*V11), "")</f>
         <v/>
       </c>
-      <c r="AC10" s="160" t="str">
+      <c r="AC10" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y10)*W11), "")</f>
         <v/>
       </c>
-      <c r="AD10" s="160" t="str">
+      <c r="AD10" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y10)*X11), "")</f>
         <v/>
       </c>
-      <c r="AE10" s="178" t="str">
+      <c r="AE10" s="194" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, SUM(AA10:AD10), "")</f>
         <v/>
       </c>
-      <c r="AF10" s="160" t="str">
+      <c r="AF10" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y10)*U11), "")</f>
         <v/>
       </c>
-      <c r="AG10" s="160" t="str">
+      <c r="AG10" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y10)*V11), "")</f>
         <v/>
       </c>
-      <c r="AH10" s="160" t="str">
+      <c r="AH10" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y10)*W11), "")</f>
         <v/>
       </c>
-      <c r="AI10" s="160" t="str">
+      <c r="AI10" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y10)*X11), "")</f>
         <v/>
       </c>
-      <c r="AJ10" s="175" t="str">
+      <c r="AJ10" s="192" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, SUM(AF10:AI10), "")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="181" t="s">
+      <c r="A11" s="197" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="181"/>
+      <c r="B11" s="197"/>
       <c r="F11" s="55">
         <v>29</v>
       </c>
@@ -2928,33 +2954,33 @@
         <f t="shared" ref="K11:K18" si="4">IFERROR(J11*BOOST_PRICE,"")</f>
         <v>240.00000000000011</v>
       </c>
-      <c r="L11" s="199" t="s">
+      <c r="L11" s="216" t="s">
         <v>13</v>
       </c>
       <c r="M11" s="55">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N11" s="134" t="s">
         <v>1</v>
       </c>
       <c r="O11" s="41">
         <f>VLOOKUP(M11, DATA_IO,6)+VLOOKUP(M12, DATA_IO,6)</f>
-        <v>16.5</v>
+        <v>17.5</v>
       </c>
       <c r="P11" s="36">
         <f t="shared" ref="P11:P18" si="5">IF(VLOOKUP(M11, DATA_IO, 8)=0, "", VLOOKUP(M11, DATA_IO, 8))</f>
-        <v>19.5</v>
+        <v>18.5</v>
       </c>
       <c r="Q11" s="99">
         <f t="shared" ref="Q11:Q18" si="6">IFERROR(P11*BOOST_PRICE,"")</f>
-        <v>2340.0000000000009</v>
+        <v>2220.0000000000009</v>
       </c>
       <c r="R11" s="71">
         <f t="shared" ref="R11:R18" si="7">VLOOKUP(M11, DATA_IO, 5, TRUE)</f>
-        <v>1280</v>
-      </c>
-      <c r="S11" s="159"/>
-      <c r="T11" s="160"/>
+        <v>1240</v>
+      </c>
+      <c r="S11" s="176"/>
+      <c r="T11" s="177"/>
       <c r="U11" s="89" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, U10/$T10, "")</f>
         <v/>
@@ -2971,22 +2997,22 @@
         <f>IF(HDRAG_HAS_REC_HJUP, X10/$T10, "")</f>
         <v/>
       </c>
-      <c r="Y11" s="165"/>
-      <c r="Z11" s="165"/>
-      <c r="AA11" s="180"/>
-      <c r="AB11" s="160"/>
-      <c r="AC11" s="160"/>
-      <c r="AD11" s="160"/>
-      <c r="AE11" s="178"/>
-      <c r="AF11" s="160"/>
-      <c r="AG11" s="160"/>
-      <c r="AH11" s="160"/>
-      <c r="AI11" s="160"/>
-      <c r="AJ11" s="175"/>
+      <c r="Y11" s="182"/>
+      <c r="Z11" s="182"/>
+      <c r="AA11" s="196"/>
+      <c r="AB11" s="177"/>
+      <c r="AC11" s="177"/>
+      <c r="AD11" s="177"/>
+      <c r="AE11" s="194"/>
+      <c r="AF11" s="177"/>
+      <c r="AG11" s="177"/>
+      <c r="AH11" s="177"/>
+      <c r="AI11" s="177"/>
+      <c r="AJ11" s="192"/>
     </row>
     <row r="12" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="181"/>
-      <c r="B12" s="181"/>
+      <c r="A12" s="197"/>
+      <c r="B12" s="197"/>
       <c r="F12" s="55">
         <v>30</v>
       </c>
@@ -3009,9 +3035,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L12" s="199"/>
+      <c r="L12" s="216"/>
       <c r="M12" s="55">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N12" s="134" t="s">
         <v>0</v>
@@ -3022,20 +3048,20 @@
       </c>
       <c r="P12" s="36">
         <f t="shared" si="5"/>
-        <v>17.416666666666668</v>
+        <v>16.25</v>
       </c>
       <c r="Q12" s="99">
         <f t="shared" si="6"/>
-        <v>2090.0000000000009</v>
+        <v>1950.0000000000009</v>
       </c>
       <c r="R12" s="30">
         <f t="shared" si="7"/>
-        <v>1180</v>
-      </c>
-      <c r="S12" s="157" t="s">
+        <v>1120</v>
+      </c>
+      <c r="S12" s="174" t="s">
         <v>59</v>
       </c>
-      <c r="T12" s="155" t="str">
+      <c r="T12" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, COUNTA(DATA_HDRAG_HZOD), "")</f>
         <v/>
       </c>
@@ -3055,59 +3081,59 @@
         <f>IF(HDRAG_HAS_REC_HZOD, COUNTIF(DATA_HDRAG_HZOD, "=5"), "")</f>
         <v/>
       </c>
-      <c r="Y12" s="166" t="str">
+      <c r="Y12" s="183" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD,AVERAGE(DATA_HDRAG_HZOD),"")</f>
         <v/>
       </c>
-      <c r="Z12" s="166"/>
-      <c r="AA12" s="163" t="str">
+      <c r="Z12" s="183"/>
+      <c r="AA12" s="180" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y12)*U13), "")</f>
         <v/>
       </c>
-      <c r="AB12" s="155" t="str">
+      <c r="AB12" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y12)*V13), "")</f>
         <v/>
       </c>
-      <c r="AC12" s="155" t="str">
+      <c r="AC12" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y12)*W13), "")</f>
         <v/>
       </c>
-      <c r="AD12" s="155" t="str">
+      <c r="AD12" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON/$Y12)*X13), "")</f>
         <v/>
       </c>
-      <c r="AE12" s="169" t="str">
+      <c r="AE12" s="186" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, SUM(AA12:AD12), "")</f>
         <v/>
       </c>
-      <c r="AF12" s="155" t="str">
+      <c r="AF12" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y12)*U13), "")</f>
         <v/>
       </c>
-      <c r="AG12" s="155" t="str">
+      <c r="AG12" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y12)*V13), "")</f>
         <v/>
       </c>
-      <c r="AH12" s="155" t="str">
+      <c r="AH12" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y12)*W13), "")</f>
         <v/>
       </c>
-      <c r="AI12" s="155" t="str">
+      <c r="AI12" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_BUILDING/$Y12)*X13), "")</f>
         <v/>
       </c>
-      <c r="AJ12" s="172" t="str">
+      <c r="AJ12" s="189" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, SUM(AF12:AI12), "")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="205" t="s">
+      <c r="A13" s="222" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="205"/>
+      <c r="B13" s="222"/>
       <c r="F13" s="56">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G13" s="133" t="s">
         <v>1</v>
@@ -3118,17 +3144,17 @@
       </c>
       <c r="I13" s="72">
         <f t="shared" si="2"/>
-        <v>780</v>
+        <v>680</v>
       </c>
       <c r="J13" s="37">
         <f t="shared" si="3"/>
-        <v>10.75</v>
+        <v>9.1666666666666661</v>
       </c>
       <c r="K13" s="31">
         <f t="shared" si="4"/>
-        <v>1290.0000000000007</v>
-      </c>
-      <c r="L13" s="216" t="s">
+        <v>1100.0000000000005</v>
+      </c>
+      <c r="L13" s="233" t="s">
         <v>7</v>
       </c>
       <c r="M13" s="56">
@@ -3153,8 +3179,8 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S13" s="158"/>
-      <c r="T13" s="156"/>
+      <c r="S13" s="175"/>
+      <c r="T13" s="173"/>
       <c r="U13" s="111" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, U12/$T12, "")</f>
         <v/>
@@ -3171,45 +3197,45 @@
         <f>IF(HDRAG_HAS_REC_HZOD, X12/$T12, "")</f>
         <v/>
       </c>
-      <c r="Y13" s="167"/>
-      <c r="Z13" s="167"/>
-      <c r="AA13" s="163"/>
-      <c r="AB13" s="155"/>
-      <c r="AC13" s="155"/>
-      <c r="AD13" s="155"/>
-      <c r="AE13" s="169"/>
-      <c r="AF13" s="155"/>
-      <c r="AG13" s="155"/>
-      <c r="AH13" s="155"/>
-      <c r="AI13" s="155"/>
-      <c r="AJ13" s="172"/>
+      <c r="Y13" s="184"/>
+      <c r="Z13" s="184"/>
+      <c r="AA13" s="180"/>
+      <c r="AB13" s="172"/>
+      <c r="AC13" s="172"/>
+      <c r="AD13" s="172"/>
+      <c r="AE13" s="186"/>
+      <c r="AF13" s="172"/>
+      <c r="AG13" s="172"/>
+      <c r="AH13" s="172"/>
+      <c r="AI13" s="172"/>
+      <c r="AJ13" s="189"/>
     </row>
     <row r="14" spans="1:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="205"/>
-      <c r="B14" s="205"/>
+      <c r="A14" s="222"/>
+      <c r="B14" s="222"/>
       <c r="F14" s="56">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G14" s="133" t="s">
         <v>0</v>
       </c>
       <c r="H14" s="42">
         <f>VLOOKUP(F13, DATA_IO,7)+VLOOKUP(F14, DATA_IO,7)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I14" s="72">
         <f t="shared" si="2"/>
-        <v>780</v>
+        <v>680</v>
       </c>
       <c r="J14" s="37">
         <f t="shared" si="3"/>
-        <v>10.75</v>
+        <v>9.1666666666666661</v>
       </c>
       <c r="K14" s="31">
         <f t="shared" si="4"/>
-        <v>1290.0000000000007</v>
-      </c>
-      <c r="L14" s="216"/>
+        <v>1100.0000000000005</v>
+      </c>
+      <c r="L14" s="233"/>
       <c r="M14" s="56">
         <v>30</v>
       </c>
@@ -3240,26 +3266,26 @@
       <c r="X14" s="128"/>
       <c r="Y14" s="128"/>
       <c r="Z14" s="128"/>
-      <c r="AA14" s="193" t="s">
+      <c r="AA14" s="210" t="s">
         <v>52</v>
       </c>
-      <c r="AB14" s="184"/>
-      <c r="AC14" s="184"/>
-      <c r="AD14" s="184"/>
-      <c r="AE14" s="184"/>
-      <c r="AF14" s="184" t="s">
+      <c r="AB14" s="200"/>
+      <c r="AC14" s="200"/>
+      <c r="AD14" s="200"/>
+      <c r="AE14" s="200"/>
+      <c r="AF14" s="200" t="s">
         <v>53</v>
       </c>
-      <c r="AG14" s="184"/>
-      <c r="AH14" s="184"/>
-      <c r="AI14" s="184"/>
-      <c r="AJ14" s="194"/>
+      <c r="AG14" s="200"/>
+      <c r="AH14" s="200"/>
+      <c r="AI14" s="200"/>
+      <c r="AJ14" s="211"/>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A15" s="204" t="s">
+      <c r="A15" s="221" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="204"/>
+      <c r="B15" s="221"/>
       <c r="F15" s="57">
         <v>29</v>
       </c>
@@ -3282,7 +3308,7 @@
         <f t="shared" si="4"/>
         <v>240.00000000000011</v>
       </c>
-      <c r="L15" s="215" t="s">
+      <c r="L15" s="232" t="s">
         <v>4</v>
       </c>
       <c r="M15" s="57">
@@ -3357,8 +3383,8 @@
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A16" s="204"/>
-      <c r="B16" s="204"/>
+      <c r="A16" s="221"/>
+      <c r="B16" s="221"/>
       <c r="F16" s="57">
         <v>30</v>
       </c>
@@ -3381,7 +3407,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L16" s="215"/>
+      <c r="L16" s="232"/>
       <c r="M16" s="57">
         <v>30</v>
       </c>
@@ -3404,12 +3430,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S16" s="168" t="s">
+      <c r="S16" s="185" t="s">
         <v>64</v>
       </c>
-      <c r="T16" s="184"/>
+      <c r="T16" s="200"/>
       <c r="U16" s="128">
-        <v>201</v>
+        <v>267</v>
       </c>
       <c r="V16" s="128"/>
       <c r="W16" s="128">
@@ -3418,52 +3444,52 @@
       <c r="X16" s="128"/>
       <c r="Y16" s="128"/>
       <c r="Z16" s="128"/>
-      <c r="AA16" s="192">
+      <c r="AA16" s="209">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y4)*U5), "")</f>
-        <v>328</v>
-      </c>
-      <c r="AB16" s="181">
+        <v>337</v>
+      </c>
+      <c r="AB16" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y4)*V5), "")</f>
-        <v>107</v>
-      </c>
-      <c r="AC16" s="181">
+        <v>103</v>
+      </c>
+      <c r="AC16" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y4)*W5), "")</f>
         <v>25</v>
       </c>
-      <c r="AD16" s="181">
+      <c r="AD16" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y4)*X5), "")</f>
-        <v>15</v>
-      </c>
-      <c r="AE16" s="195">
+        <v>13</v>
+      </c>
+      <c r="AE16" s="212">
         <f>IF(HDRAG_HAS_REC_HBRUN, SUM(AA16:AD16), "")</f>
-        <v>475</v>
-      </c>
-      <c r="AF16" s="181">
+        <v>478</v>
+      </c>
+      <c r="AF16" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y4)*U5), "")</f>
-        <v>372</v>
-      </c>
-      <c r="AG16" s="181">
+        <v>383</v>
+      </c>
+      <c r="AG16" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y4)*V5), "")</f>
-        <v>122</v>
-      </c>
-      <c r="AH16" s="181">
+        <v>117</v>
+      </c>
+      <c r="AH16" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y4)*W5), "")</f>
         <v>29</v>
       </c>
-      <c r="AI16" s="181">
+      <c r="AI16" s="197">
         <f>IF(HDRAG_HAS_REC_HBRUN, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y4)*X5), "")</f>
-        <v>17</v>
-      </c>
-      <c r="AJ16" s="185">
+        <v>15</v>
+      </c>
+      <c r="AJ16" s="201">
         <f>IF(HDRAG_HAS_REC_HBRUN, SUM(AF16:AI16), "")</f>
-        <v>540</v>
+        <v>544</v>
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A17" s="203" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="203"/>
+      <c r="A17" s="220" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="220"/>
       <c r="F17" s="58">
         <v>30</v>
       </c>
@@ -3486,7 +3512,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L17" s="157" t="s">
+      <c r="L17" s="174" t="s">
         <v>2</v>
       </c>
       <c r="M17" s="59">
@@ -3511,7 +3537,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S17" s="168" t="s">
+      <c r="S17" s="185" t="s">
         <v>60</v>
       </c>
       <c r="T17" s="125" t="s">
@@ -3527,20 +3553,20 @@
       <c r="X17" s="128"/>
       <c r="Y17" s="128"/>
       <c r="Z17" s="128"/>
-      <c r="AA17" s="192"/>
-      <c r="AB17" s="181"/>
-      <c r="AC17" s="181"/>
-      <c r="AD17" s="181"/>
-      <c r="AE17" s="195"/>
-      <c r="AF17" s="181"/>
-      <c r="AG17" s="181"/>
-      <c r="AH17" s="181"/>
-      <c r="AI17" s="181"/>
-      <c r="AJ17" s="185"/>
+      <c r="AA17" s="209"/>
+      <c r="AB17" s="197"/>
+      <c r="AC17" s="197"/>
+      <c r="AD17" s="197"/>
+      <c r="AE17" s="212"/>
+      <c r="AF17" s="197"/>
+      <c r="AG17" s="197"/>
+      <c r="AH17" s="197"/>
+      <c r="AI17" s="197"/>
+      <c r="AJ17" s="201"/>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A18" s="203"/>
-      <c r="B18" s="203"/>
+      <c r="A18" s="220"/>
+      <c r="B18" s="220"/>
       <c r="F18" s="58">
         <v>30</v>
       </c>
@@ -3563,7 +3589,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L18" s="157"/>
+      <c r="L18" s="174"/>
       <c r="M18" s="59">
         <v>30</v>
       </c>
@@ -3586,7 +3612,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S18" s="168"/>
+      <c r="S18" s="185"/>
       <c r="T18" s="125" t="s">
         <v>36</v>
       </c>
@@ -3611,43 +3637,43 @@
         <v/>
       </c>
       <c r="Z18" s="128"/>
-      <c r="AA18" s="187" t="str">
+      <c r="AA18" s="203" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y6)*U7), "")</f>
         <v/>
       </c>
-      <c r="AB18" s="176" t="str">
+      <c r="AB18" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y6)*V7), "")</f>
         <v/>
       </c>
-      <c r="AC18" s="176" t="str">
+      <c r="AC18" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y6)*W7), "")</f>
         <v/>
       </c>
-      <c r="AD18" s="176" t="str">
+      <c r="AD18" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y6)*X7), "")</f>
         <v/>
       </c>
-      <c r="AE18" s="177" t="str">
+      <c r="AE18" s="204" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, SUM(AA18:AD18), "")</f>
         <v/>
       </c>
-      <c r="AF18" s="176" t="str">
+      <c r="AF18" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y6)*U7), "")</f>
         <v/>
       </c>
-      <c r="AG18" s="176" t="str">
+      <c r="AG18" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y6)*V7), "")</f>
         <v/>
       </c>
-      <c r="AH18" s="176" t="str">
+      <c r="AH18" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y6)*W7), "")</f>
         <v/>
       </c>
-      <c r="AI18" s="176" t="str">
+      <c r="AI18" s="193" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y6)*X7), "")</f>
         <v/>
       </c>
-      <c r="AJ18" s="186" t="str">
+      <c r="AJ18" s="202" t="str">
         <f>IF(HDRAG_HAS_REC_HMERC, SUM(AF18:AI18), "")</f>
         <v/>
       </c>
@@ -3662,7 +3688,7 @@
       <c r="J19" s="64"/>
       <c r="K19" s="1"/>
       <c r="Q19" s="97"/>
-      <c r="S19" s="168" t="s">
+      <c r="S19" s="185" t="s">
         <v>63</v>
       </c>
       <c r="T19" s="125" t="s">
@@ -3671,44 +3697,44 @@
       <c r="W19" s="128">
         <v>4</v>
       </c>
-      <c r="AA19" s="187"/>
-      <c r="AB19" s="176"/>
-      <c r="AC19" s="176"/>
-      <c r="AD19" s="176"/>
-      <c r="AE19" s="177"/>
-      <c r="AF19" s="176"/>
-      <c r="AG19" s="176"/>
-      <c r="AH19" s="176"/>
-      <c r="AI19" s="176"/>
-      <c r="AJ19" s="186"/>
+      <c r="AA19" s="203"/>
+      <c r="AB19" s="193"/>
+      <c r="AC19" s="193"/>
+      <c r="AD19" s="193"/>
+      <c r="AE19" s="204"/>
+      <c r="AF19" s="193"/>
+      <c r="AG19" s="193"/>
+      <c r="AH19" s="193"/>
+      <c r="AI19" s="193"/>
+      <c r="AJ19" s="202"/>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B20" s="206" t="s">
+      <c r="B20" s="223" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="206"/>
-      <c r="D20" s="206"/>
-      <c r="E20" s="206"/>
-      <c r="F20" s="206"/>
-      <c r="G20" s="211">
+      <c r="C20" s="223"/>
+      <c r="D20" s="223"/>
+      <c r="E20" s="223"/>
+      <c r="F20" s="223"/>
+      <c r="G20" s="228">
         <f>SUM(J11:J18,P11:P18)</f>
-        <v>62.416666666666671</v>
-      </c>
-      <c r="H20" s="211"/>
-      <c r="I20" s="211"/>
-      <c r="J20" s="211"/>
-      <c r="K20" s="206" t="s">
+        <v>57.083333333333329</v>
+      </c>
+      <c r="H20" s="228"/>
+      <c r="I20" s="228"/>
+      <c r="J20" s="228"/>
+      <c r="K20" s="223" t="s">
         <v>32</v>
       </c>
-      <c r="L20" s="206"/>
-      <c r="M20" s="213">
+      <c r="L20" s="223"/>
+      <c r="M20" s="230">
         <f>SUM(K11:K18,Q11:Q18)</f>
-        <v>7490.0000000000036</v>
-      </c>
-      <c r="N20" s="213"/>
-      <c r="O20" s="213"/>
+        <v>6850.0000000000027</v>
+      </c>
+      <c r="N20" s="230"/>
+      <c r="O20" s="230"/>
       <c r="Q20" s="97"/>
-      <c r="S20" s="168"/>
+      <c r="S20" s="185"/>
       <c r="T20" s="125" t="s">
         <v>36</v>
       </c>
@@ -3733,73 +3759,73 @@
         <v/>
       </c>
       <c r="Z20" s="128"/>
-      <c r="AA20" s="171">
+      <c r="AA20" s="188">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y8)*U9), "")</f>
         <v>292</v>
       </c>
-      <c r="AB20" s="162">
+      <c r="AB20" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y8)*V9), "")</f>
         <v>96</v>
       </c>
-      <c r="AC20" s="162">
+      <c r="AC20" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y8)*W9), "")</f>
         <v>35</v>
       </c>
-      <c r="AD20" s="162">
+      <c r="AD20" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y8)*X9), "")</f>
         <v>28</v>
       </c>
-      <c r="AE20" s="161">
+      <c r="AE20" s="178">
         <f>IF(HDRAG_HAS_REC_HMID, SUM(AA20:AD20), "")</f>
         <v>451</v>
       </c>
-      <c r="AF20" s="162">
+      <c r="AF20" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y8)*U9), "")</f>
         <v>332</v>
       </c>
-      <c r="AG20" s="162">
+      <c r="AG20" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y8)*V9), "")</f>
         <v>108</v>
       </c>
-      <c r="AH20" s="162">
+      <c r="AH20" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y8)*W9), "")</f>
         <v>40</v>
       </c>
-      <c r="AI20" s="162">
+      <c r="AI20" s="179">
         <f>IF(HDRAG_HAS_REC_HMID, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y8)*X9), "")</f>
         <v>32</v>
       </c>
-      <c r="AJ20" s="179">
+      <c r="AJ20" s="195">
         <f>IF(HDRAG_HAS_REC_HMID, SUM(AF20:AI20), "")</f>
         <v>512</v>
       </c>
     </row>
     <row r="21" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="129"/>
-      <c r="B21" s="207"/>
-      <c r="C21" s="207"/>
-      <c r="D21" s="207"/>
-      <c r="E21" s="207"/>
-      <c r="F21" s="207"/>
-      <c r="G21" s="212"/>
-      <c r="H21" s="212"/>
-      <c r="I21" s="212"/>
-      <c r="J21" s="212"/>
-      <c r="K21" s="207"/>
-      <c r="L21" s="207"/>
-      <c r="M21" s="214"/>
-      <c r="N21" s="214"/>
-      <c r="O21" s="214"/>
+      <c r="B21" s="224"/>
+      <c r="C21" s="224"/>
+      <c r="D21" s="224"/>
+      <c r="E21" s="224"/>
+      <c r="F21" s="224"/>
+      <c r="G21" s="229"/>
+      <c r="H21" s="229"/>
+      <c r="I21" s="229"/>
+      <c r="J21" s="229"/>
+      <c r="K21" s="224"/>
+      <c r="L21" s="224"/>
+      <c r="M21" s="231"/>
+      <c r="N21" s="231"/>
+      <c r="O21" s="231"/>
       <c r="P21" s="129"/>
       <c r="Q21" s="67"/>
       <c r="R21" s="66"/>
-      <c r="S21" s="168" t="s">
+      <c r="S21" s="185" t="s">
         <v>65</v>
       </c>
-      <c r="T21" s="184"/>
+      <c r="T21" s="200"/>
       <c r="U21" s="128">
         <f>IFERROR(IF(U18+U20=0,0,U18+U20-U16), "")</f>
-        <v>704</v>
+        <v>638</v>
       </c>
       <c r="V21" s="128" t="str">
         <f>IFERROR(IF(V18+V20=0,0,V18+V20-V16), "")</f>
@@ -3818,38 +3844,38 @@
         <v/>
       </c>
       <c r="Z21" s="128"/>
-      <c r="AA21" s="171"/>
-      <c r="AB21" s="162"/>
-      <c r="AC21" s="162"/>
-      <c r="AD21" s="162"/>
-      <c r="AE21" s="161"/>
-      <c r="AF21" s="162"/>
-      <c r="AG21" s="162"/>
-      <c r="AH21" s="162"/>
-      <c r="AI21" s="162"/>
-      <c r="AJ21" s="179"/>
+      <c r="AA21" s="188"/>
+      <c r="AB21" s="179"/>
+      <c r="AC21" s="179"/>
+      <c r="AD21" s="179"/>
+      <c r="AE21" s="178"/>
+      <c r="AF21" s="179"/>
+      <c r="AG21" s="179"/>
+      <c r="AH21" s="179"/>
+      <c r="AI21" s="179"/>
+      <c r="AJ21" s="195"/>
     </row>
     <row r="22" spans="1:36" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="209" t="s">
+      <c r="A22" s="226" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="209"/>
-      <c r="C22" s="209"/>
-      <c r="D22" s="209"/>
-      <c r="E22" s="209"/>
-      <c r="F22" s="209"/>
-      <c r="G22" s="209"/>
-      <c r="H22" s="209"/>
-      <c r="I22" s="209"/>
-      <c r="J22" s="209"/>
-      <c r="K22" s="209"/>
-      <c r="L22" s="209"/>
-      <c r="M22" s="209"/>
-      <c r="N22" s="209"/>
-      <c r="O22" s="209"/>
-      <c r="P22" s="209"/>
-      <c r="Q22" s="210"/>
-      <c r="S22" s="168" t="s">
+      <c r="B22" s="226"/>
+      <c r="C22" s="226"/>
+      <c r="D22" s="226"/>
+      <c r="E22" s="226"/>
+      <c r="F22" s="226"/>
+      <c r="G22" s="226"/>
+      <c r="H22" s="226"/>
+      <c r="I22" s="226"/>
+      <c r="J22" s="226"/>
+      <c r="K22" s="226"/>
+      <c r="L22" s="226"/>
+      <c r="M22" s="226"/>
+      <c r="N22" s="226"/>
+      <c r="O22" s="226"/>
+      <c r="P22" s="226"/>
+      <c r="Q22" s="227"/>
+      <c r="S22" s="185" t="s">
         <v>38</v>
       </c>
       <c r="T22" s="125">
@@ -3857,7 +3883,7 @@
       </c>
       <c r="U22" s="128">
         <f>IFERROR(IF(U$21=0, "", _xlfn.CEILING.MATH((U$21/Y4)*U5)),"")</f>
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="V22" s="128" t="str">
         <f>IFERROR(IF(V$21=0, "", _xlfn.CEILING.MATH((V$21/Y6)*U7)),"")</f>
@@ -3876,72 +3902,72 @@
         <v/>
       </c>
       <c r="Z22" s="110"/>
-      <c r="AA22" s="160" t="str">
+      <c r="AA22" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y10)*U11), "")</f>
         <v/>
       </c>
-      <c r="AB22" s="160" t="str">
+      <c r="AB22" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y10)*V11), "")</f>
         <v/>
       </c>
-      <c r="AC22" s="160" t="str">
+      <c r="AC22" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y10)*W11), "")</f>
         <v/>
       </c>
-      <c r="AD22" s="160" t="str">
+      <c r="AD22" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y10)*X11), "")</f>
         <v/>
       </c>
-      <c r="AE22" s="178" t="str">
+      <c r="AE22" s="194" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, SUM(AA22:AD22), "")</f>
         <v/>
       </c>
-      <c r="AF22" s="160" t="str">
+      <c r="AF22" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y10)*U11), "")</f>
         <v/>
       </c>
-      <c r="AG22" s="160" t="str">
+      <c r="AG22" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y10)*V11), "")</f>
         <v/>
       </c>
-      <c r="AH22" s="160" t="str">
+      <c r="AH22" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y10)*W11), "")</f>
         <v/>
       </c>
-      <c r="AI22" s="160" t="str">
+      <c r="AI22" s="177" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y10)*X11), "")</f>
         <v/>
       </c>
-      <c r="AJ22" s="175" t="str">
+      <c r="AJ22" s="192" t="str">
         <f>IF(HDRAG_HAS_REC_HJUP, SUM(AF22:AI22), "")</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="201"/>
-      <c r="B23" s="201"/>
-      <c r="C23" s="201"/>
-      <c r="D23" s="201"/>
-      <c r="E23" s="201"/>
-      <c r="F23" s="201"/>
-      <c r="G23" s="201"/>
-      <c r="H23" s="201"/>
-      <c r="I23" s="201"/>
-      <c r="J23" s="201"/>
-      <c r="K23" s="201"/>
-      <c r="L23" s="201"/>
-      <c r="M23" s="201"/>
-      <c r="N23" s="201"/>
-      <c r="O23" s="201"/>
-      <c r="P23" s="201"/>
-      <c r="Q23" s="202"/>
-      <c r="S23" s="168"/>
+      <c r="A23" s="218"/>
+      <c r="B23" s="218"/>
+      <c r="C23" s="218"/>
+      <c r="D23" s="218"/>
+      <c r="E23" s="218"/>
+      <c r="F23" s="218"/>
+      <c r="G23" s="218"/>
+      <c r="H23" s="218"/>
+      <c r="I23" s="218"/>
+      <c r="J23" s="218"/>
+      <c r="K23" s="218"/>
+      <c r="L23" s="218"/>
+      <c r="M23" s="218"/>
+      <c r="N23" s="218"/>
+      <c r="O23" s="218"/>
+      <c r="P23" s="218"/>
+      <c r="Q23" s="219"/>
+      <c r="S23" s="185"/>
       <c r="T23" s="125">
         <v>3</v>
       </c>
       <c r="U23" s="128">
         <f>IFERROR(IF(U$21=0, "", _xlfn.CEILING.MATH((U$21/Y4)*V5)),"")</f>
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="V23" s="128" t="str">
         <f>IFERROR(IF(V$21=0, "", _xlfn.CEILING.MATH((V$21/Y6)*V7)),"")</f>
@@ -3960,42 +3986,42 @@
         <v/>
       </c>
       <c r="Z23" s="110"/>
-      <c r="AA23" s="160"/>
-      <c r="AB23" s="160"/>
-      <c r="AC23" s="160"/>
-      <c r="AD23" s="160"/>
-      <c r="AE23" s="178"/>
-      <c r="AF23" s="160"/>
-      <c r="AG23" s="160"/>
-      <c r="AH23" s="160"/>
-      <c r="AI23" s="160"/>
-      <c r="AJ23" s="175"/>
+      <c r="AA23" s="177"/>
+      <c r="AB23" s="177"/>
+      <c r="AC23" s="177"/>
+      <c r="AD23" s="177"/>
+      <c r="AE23" s="194"/>
+      <c r="AF23" s="177"/>
+      <c r="AG23" s="177"/>
+      <c r="AH23" s="177"/>
+      <c r="AI23" s="177"/>
+      <c r="AJ23" s="192"/>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A24" s="201"/>
-      <c r="B24" s="201"/>
-      <c r="C24" s="201"/>
-      <c r="D24" s="201"/>
-      <c r="E24" s="201"/>
-      <c r="F24" s="201"/>
-      <c r="G24" s="201"/>
-      <c r="H24" s="201"/>
-      <c r="I24" s="201"/>
-      <c r="J24" s="201"/>
-      <c r="K24" s="201"/>
-      <c r="L24" s="201"/>
-      <c r="M24" s="201"/>
-      <c r="N24" s="201"/>
-      <c r="O24" s="201"/>
-      <c r="P24" s="201"/>
-      <c r="Q24" s="202"/>
-      <c r="S24" s="168"/>
+      <c r="A24" s="218"/>
+      <c r="B24" s="218"/>
+      <c r="C24" s="218"/>
+      <c r="D24" s="218"/>
+      <c r="E24" s="218"/>
+      <c r="F24" s="218"/>
+      <c r="G24" s="218"/>
+      <c r="H24" s="218"/>
+      <c r="I24" s="218"/>
+      <c r="J24" s="218"/>
+      <c r="K24" s="218"/>
+      <c r="L24" s="218"/>
+      <c r="M24" s="218"/>
+      <c r="N24" s="218"/>
+      <c r="O24" s="218"/>
+      <c r="P24" s="218"/>
+      <c r="Q24" s="219"/>
+      <c r="S24" s="185"/>
       <c r="T24" s="125">
         <v>4</v>
       </c>
       <c r="U24" s="128">
         <f>IFERROR(IF(U$21=0, "", _xlfn.CEILING.MATH((U$21/Y4)*W5)),"")</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="V24" s="128" t="str">
         <f>IFERROR(IF(V$21=0, "", _xlfn.CEILING.MATH((V$21/Y6)*W7)),"")</f>
@@ -4014,78 +4040,78 @@
         <v/>
       </c>
       <c r="Z24" s="110"/>
-      <c r="AA24" s="163" t="str">
+      <c r="AA24" s="180" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y12)*U13), "")</f>
         <v/>
       </c>
-      <c r="AB24" s="155" t="str">
+      <c r="AB24" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y12)*V13), "")</f>
         <v/>
       </c>
-      <c r="AC24" s="155" t="str">
+      <c r="AC24" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y12)*W13), "")</f>
         <v/>
       </c>
-      <c r="AD24" s="155" t="str">
+      <c r="AD24" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_DRAGON_BLD_16/$Y12)*X13), "")</f>
         <v/>
       </c>
-      <c r="AE24" s="169" t="str">
+      <c r="AE24" s="186" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, SUM(AA24:AD24), "")</f>
         <v/>
       </c>
-      <c r="AF24" s="155" t="str">
+      <c r="AF24" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y12)*U13), "")</f>
         <v/>
       </c>
-      <c r="AG24" s="155" t="str">
+      <c r="AG24" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y12)*V13), "")</f>
         <v/>
       </c>
-      <c r="AH24" s="155" t="str">
+      <c r="AH24" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y12)*W13), "")</f>
         <v/>
       </c>
-      <c r="AI24" s="155" t="str">
+      <c r="AI24" s="172" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, _xlfn.CEILING.MATH((HDRAGS_MAX_ALL/$Y12)*X13), "")</f>
         <v/>
       </c>
-      <c r="AJ24" s="172" t="str">
+      <c r="AJ24" s="189" t="str">
         <f>IF(HDRAG_HAS_REC_HZOD, SUM(AF24:AI24), "")</f>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="128"/>
-      <c r="B25" s="184" t="s">
+      <c r="B25" s="200" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="184"/>
-      <c r="D25" s="184"/>
-      <c r="E25" s="184"/>
-      <c r="F25" s="184"/>
-      <c r="G25" s="184"/>
+      <c r="C25" s="200"/>
+      <c r="D25" s="200"/>
+      <c r="E25" s="200"/>
+      <c r="F25" s="200"/>
+      <c r="G25" s="200"/>
       <c r="H25" s="128"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="198" t="s">
+      <c r="J25" s="215" t="s">
         <v>82</v>
       </c>
-      <c r="K25" s="198"/>
+      <c r="K25" s="215"/>
       <c r="L25" s="49"/>
-      <c r="M25" s="198" t="s">
+      <c r="M25" s="215" t="s">
         <v>84</v>
       </c>
-      <c r="N25" s="198"/>
-      <c r="O25" s="198"/>
-      <c r="P25" s="198"/>
+      <c r="N25" s="215"/>
+      <c r="O25" s="215"/>
+      <c r="P25" s="215"/>
       <c r="Q25" s="97"/>
-      <c r="S25" s="168"/>
+      <c r="S25" s="185"/>
       <c r="T25" s="125">
         <v>5</v>
       </c>
       <c r="U25" s="128">
         <f>IFERROR(IF(U$21=0, "", _xlfn.CEILING.MATH((U$21/Y4)*X5)),"")</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="V25" s="128" t="str">
         <f>IFERROR(IF(V$21=0, "", _xlfn.CEILING.MATH((V$21/Y6)*X7)),"")</f>
@@ -4104,56 +4130,56 @@
         <v/>
       </c>
       <c r="Z25" s="110"/>
-      <c r="AA25" s="174"/>
-      <c r="AB25" s="156"/>
-      <c r="AC25" s="156"/>
-      <c r="AD25" s="156"/>
-      <c r="AE25" s="170"/>
-      <c r="AF25" s="156"/>
-      <c r="AG25" s="156"/>
-      <c r="AH25" s="156"/>
-      <c r="AI25" s="156"/>
-      <c r="AJ25" s="173"/>
+      <c r="AA25" s="191"/>
+      <c r="AB25" s="173"/>
+      <c r="AC25" s="173"/>
+      <c r="AD25" s="173"/>
+      <c r="AE25" s="187"/>
+      <c r="AF25" s="173"/>
+      <c r="AG25" s="173"/>
+      <c r="AH25" s="173"/>
+      <c r="AI25" s="173"/>
+      <c r="AJ25" s="190"/>
     </row>
     <row r="26" spans="1:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="128"/>
-      <c r="B26" s="184" t="s">
+      <c r="B26" s="200" t="s">
         <v>70</v>
       </c>
       <c r="C26" s="63"/>
       <c r="D26" s="63"/>
       <c r="E26" s="63"/>
-      <c r="F26" s="227">
-        <v>8186</v>
-      </c>
-      <c r="G26" s="227"/>
+      <c r="F26" s="240">
+        <v>9734</v>
+      </c>
+      <c r="G26" s="240"/>
       <c r="H26" s="128"/>
       <c r="I26" s="49">
         <f>IF(K26&gt;100,100,IF(K26&lt;0,0,K26))</f>
         <v>0</v>
       </c>
-      <c r="J26" s="198" t="s">
+      <c r="J26" s="215" t="s">
         <v>61</v>
       </c>
-      <c r="K26" s="227"/>
+      <c r="K26" s="240"/>
       <c r="L26" s="128"/>
-      <c r="M26" s="198" t="s">
+      <c r="M26" s="215" t="s">
         <v>85</v>
       </c>
-      <c r="N26" s="198"/>
-      <c r="O26" s="226">
+      <c r="N26" s="215"/>
+      <c r="O26" s="239">
         <f>_xlfn.FLOOR.MATH(F32/MAX(DATA_DRAG_ACCU_EXP))</f>
         <v>1</v>
       </c>
-      <c r="P26" s="226"/>
+      <c r="P26" s="239"/>
       <c r="Q26" s="97"/>
-      <c r="S26" s="168"/>
+      <c r="S26" s="185"/>
       <c r="T26" s="125" t="s">
         <v>56</v>
       </c>
       <c r="U26" s="128">
         <f>IF(AND(HDRAG_HAS_REC_HBRUN,U21&gt;0),SUM(U22:U25),"")</f>
-        <v>293</v>
+        <v>267</v>
       </c>
       <c r="V26" s="128" t="str">
         <f>IF(AND(HDRAG_HAS_REC_HMERC,V21&gt;0),SUM(V22:V25),"")</f>
@@ -4184,26 +4210,26 @@
     </row>
     <row r="27" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="128"/>
-      <c r="B27" s="184"/>
+      <c r="B27" s="200"/>
       <c r="C27" s="63"/>
       <c r="D27" s="63"/>
       <c r="E27" s="63"/>
-      <c r="F27" s="227"/>
-      <c r="G27" s="227"/>
+      <c r="F27" s="240"/>
+      <c r="G27" s="240"/>
       <c r="H27" s="128"/>
       <c r="I27" s="49">
         <f>MOD(F32,MAX(DATA_DRAG_ACCU_EXP))</f>
-        <v>6380</v>
-      </c>
-      <c r="J27" s="198"/>
-      <c r="K27" s="227"/>
+        <v>716080</v>
+      </c>
+      <c r="J27" s="215"/>
+      <c r="K27" s="240"/>
       <c r="L27" s="128"/>
-      <c r="M27" s="198"/>
-      <c r="N27" s="198"/>
-      <c r="O27" s="226"/>
-      <c r="P27" s="226"/>
+      <c r="M27" s="215"/>
+      <c r="N27" s="215"/>
+      <c r="O27" s="239"/>
+      <c r="P27" s="239"/>
       <c r="Q27" s="97"/>
-      <c r="S27" s="182" t="s">
+      <c r="S27" s="198" t="s">
         <v>37</v>
       </c>
       <c r="T27" s="125" t="s">
@@ -4242,37 +4268,37 @@
     </row>
     <row r="28" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="128"/>
-      <c r="B28" s="184" t="s">
+      <c r="B28" s="200" t="s">
         <v>71</v>
       </c>
       <c r="C28" s="63"/>
       <c r="D28" s="63"/>
       <c r="E28" s="63"/>
-      <c r="F28" s="227">
-        <v>8</v>
-      </c>
-      <c r="G28" s="227"/>
+      <c r="F28" s="240">
+        <v>342</v>
+      </c>
+      <c r="G28" s="240"/>
       <c r="H28" s="128"/>
       <c r="I28" s="49">
         <f>SMALL(DATA_DRAG_ACCU_EXP,COUNTIF(DATA_DRAG_ACCU_EXP,"&lt;"&amp;I27))</f>
-        <v>6000</v>
-      </c>
-      <c r="J28" s="198" t="s">
+        <v>697260</v>
+      </c>
+      <c r="J28" s="215" t="s">
         <v>83</v>
       </c>
-      <c r="K28" s="227"/>
+      <c r="K28" s="240"/>
       <c r="L28" s="128"/>
-      <c r="M28" s="198" t="s">
+      <c r="M28" s="215" t="s">
         <v>61</v>
       </c>
-      <c r="N28" s="198"/>
-      <c r="O28" s="226">
+      <c r="N28" s="215"/>
+      <c r="O28" s="239">
         <f>MATCH(I28, DATA_DRAG_ACCU_EXP,0)</f>
-        <v>12</v>
-      </c>
-      <c r="P28" s="226"/>
+        <v>83</v>
+      </c>
+      <c r="P28" s="239"/>
       <c r="Q28" s="107"/>
-      <c r="S28" s="182"/>
+      <c r="S28" s="198"/>
       <c r="T28" s="125" t="s">
         <v>60</v>
       </c>
@@ -4309,32 +4335,32 @@
     </row>
     <row r="29" spans="1:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="128"/>
-      <c r="B29" s="184"/>
+      <c r="B29" s="200"/>
       <c r="C29" s="63"/>
       <c r="D29" s="63"/>
       <c r="E29" s="63"/>
-      <c r="F29" s="227"/>
-      <c r="G29" s="227"/>
+      <c r="F29" s="240"/>
+      <c r="G29" s="240"/>
       <c r="H29" s="128"/>
       <c r="I29" s="49">
         <f>IF(I26=0,0,INDEX(DATA_DRAG_ACCU_EXP,I26)+INDEX(DATA_DRAG_LV_EXP,I26)-K28)</f>
         <v>0</v>
       </c>
-      <c r="J29" s="198"/>
-      <c r="K29" s="227"/>
+      <c r="J29" s="215"/>
+      <c r="K29" s="240"/>
       <c r="L29" s="49"/>
-      <c r="M29" s="198"/>
-      <c r="N29" s="198"/>
-      <c r="O29" s="226"/>
-      <c r="P29" s="226"/>
+      <c r="M29" s="215"/>
+      <c r="N29" s="215"/>
+      <c r="O29" s="239"/>
+      <c r="P29" s="239"/>
       <c r="Q29" s="107"/>
-      <c r="S29" s="183"/>
+      <c r="S29" s="199"/>
       <c r="T29" s="103" t="s">
         <v>66</v>
       </c>
       <c r="U29" s="104">
         <f>IFERROR(IF(U21=0, 100%, (HDRAGS_MAX_ALL - U21)/HDRAGS_MAX_ALL),"")</f>
-        <v>0.45887778631821674</v>
+        <v>0.50960799385088396</v>
       </c>
       <c r="V29" s="104" t="str">
         <f>IFERROR(IF(V21=0, 100%, (HDRAGS_MAX_ALL - V21)/HDRAGS_MAX_ALL),"")</f>
@@ -4366,105 +4392,111 @@
     </row>
     <row r="30" spans="1:36" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="128"/>
-      <c r="B30" s="184" t="s">
+      <c r="B30" s="200" t="s">
         <v>72</v>
       </c>
       <c r="C30" s="63"/>
       <c r="D30" s="63"/>
       <c r="E30" s="63"/>
-      <c r="F30" s="227">
-        <v>3</v>
-      </c>
-      <c r="G30" s="227"/>
+      <c r="F30" s="240">
+        <v>44</v>
+      </c>
+      <c r="G30" s="240"/>
       <c r="H30" s="128"/>
       <c r="I30" s="1"/>
       <c r="J30" s="128"/>
       <c r="K30" s="128"/>
       <c r="L30" s="128"/>
-      <c r="M30" s="184" t="s">
+      <c r="M30" s="200" t="s">
         <v>83</v>
       </c>
-      <c r="N30" s="184"/>
-      <c r="O30" s="226">
+      <c r="N30" s="200"/>
+      <c r="O30" s="239">
         <f>INDEX(DATA_DRAG_LV_EXP,O28)-(I27-I28)</f>
-        <v>640</v>
-      </c>
-      <c r="P30" s="226"/>
+        <v>6710</v>
+      </c>
+      <c r="P30" s="239"/>
       <c r="Q30" s="107"/>
-      <c r="S30" s="218" t="s">
+      <c r="S30" s="168" t="s">
         <v>103</v>
       </c>
-      <c r="T30" s="219"/>
-      <c r="U30" s="219"/>
-      <c r="V30" s="219"/>
-      <c r="W30" s="219"/>
-      <c r="X30" s="219"/>
-      <c r="Y30" s="219"/>
+      <c r="T30" s="169"/>
+      <c r="U30" s="169"/>
+      <c r="V30" s="169"/>
+      <c r="W30" s="169"/>
+      <c r="X30" s="160"/>
+      <c r="Y30" s="160"/>
+      <c r="Z30" s="161"/>
+      <c r="AA30" s="162"/>
     </row>
     <row r="31" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="128"/>
-      <c r="B31" s="184"/>
+      <c r="B31" s="200"/>
       <c r="C31" s="63"/>
       <c r="D31" s="63"/>
       <c r="E31" s="63"/>
-      <c r="F31" s="227"/>
-      <c r="G31" s="227"/>
-      <c r="M31" s="184"/>
-      <c r="N31" s="184"/>
-      <c r="O31" s="226"/>
-      <c r="P31" s="226"/>
+      <c r="F31" s="240"/>
+      <c r="G31" s="240"/>
+      <c r="M31" s="200"/>
+      <c r="N31" s="200"/>
+      <c r="O31" s="239"/>
+      <c r="P31" s="239"/>
       <c r="Q31" s="128"/>
-      <c r="S31" s="220"/>
-      <c r="T31" s="221"/>
-      <c r="U31" s="221"/>
-      <c r="V31" s="221"/>
-      <c r="W31" s="221"/>
-      <c r="X31" s="221"/>
-      <c r="Y31" s="221"/>
+      <c r="S31" s="170"/>
+      <c r="T31" s="171"/>
+      <c r="U31" s="171"/>
+      <c r="V31" s="171"/>
+      <c r="W31" s="171"/>
+      <c r="X31" s="163"/>
+      <c r="Y31" s="163"/>
+      <c r="Z31" s="161"/>
+      <c r="AA31" s="162"/>
     </row>
     <row r="32" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="128"/>
-      <c r="B32" s="184" t="s">
+      <c r="B32" s="200" t="s">
         <v>81</v>
       </c>
       <c r="C32" s="63"/>
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
-      <c r="F32" s="224">
+      <c r="F32" s="237">
         <f>F26*DRAGEXP_S+F28*DRAGEXP_M+F30*DRAGEXP_L</f>
-        <v>1246400</v>
-      </c>
-      <c r="G32" s="224"/>
+        <v>1956100</v>
+      </c>
+      <c r="G32" s="237"/>
       <c r="M32" s="128"/>
       <c r="N32" s="128"/>
       <c r="O32" s="128"/>
       <c r="P32" s="128"/>
       <c r="Q32" s="128"/>
-      <c r="S32" s="220"/>
-      <c r="T32" s="221"/>
-      <c r="U32" s="221"/>
-      <c r="V32" s="221"/>
-      <c r="W32" s="221"/>
-      <c r="X32" s="221"/>
-      <c r="Y32" s="221"/>
-    </row>
-    <row r="33" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S32" s="170"/>
+      <c r="T32" s="171"/>
+      <c r="U32" s="171"/>
+      <c r="V32" s="171"/>
+      <c r="W32" s="171"/>
+      <c r="X32" s="163"/>
+      <c r="Y32" s="163"/>
+      <c r="Z32" s="161"/>
+      <c r="AA32" s="162"/>
+    </row>
+    <row r="33" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="128"/>
-      <c r="B33" s="184"/>
+      <c r="B33" s="200"/>
       <c r="C33" s="63"/>
       <c r="D33" s="63"/>
       <c r="E33" s="63"/>
-      <c r="F33" s="224"/>
-      <c r="G33" s="224"/>
-      <c r="J33" s="217" t="s">
+      <c r="F33" s="237"/>
+      <c r="G33" s="237"/>
+      <c r="J33" s="234" t="s">
         <v>79</v>
       </c>
-      <c r="K33" s="225">
+      <c r="K33" s="238">
         <f>IF(N34 &gt; 0, SUM(DATA_DRAGON_EXP)/N34, 0)</f>
-        <v>2615.916955017301</v>
-      </c>
-      <c r="L33" s="225"/>
-      <c r="M33" s="225"/>
+        <v>2673.9277652370201</v>
+      </c>
+      <c r="L33" s="238"/>
+      <c r="M33" s="238"/>
       <c r="N33" s="125" t="s">
         <v>42</v>
       </c>
@@ -4472,8 +4504,12 @@
       <c r="P33" s="128"/>
       <c r="Q33" s="128"/>
       <c r="S33" s="108"/>
-    </row>
-    <row r="34" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X33" s="164"/>
+      <c r="Y33" s="164"/>
+      <c r="Z33" s="161"/>
+      <c r="AA33" s="162"/>
+    </row>
+    <row r="34" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="128"/>
       <c r="B34" s="125"/>
       <c r="C34" s="63"/>
@@ -4481,13 +4517,13 @@
       <c r="E34" s="63"/>
       <c r="F34" s="126"/>
       <c r="G34" s="126"/>
-      <c r="J34" s="217"/>
-      <c r="K34" s="225"/>
-      <c r="L34" s="225"/>
-      <c r="M34" s="225"/>
+      <c r="J34" s="234"/>
+      <c r="K34" s="238"/>
+      <c r="L34" s="238"/>
+      <c r="M34" s="238"/>
       <c r="N34" s="128">
         <f>SUM(DATA_DRAGON_PLAYS)</f>
-        <v>289</v>
+        <v>443</v>
       </c>
       <c r="O34" s="128"/>
       <c r="P34" s="128"/>
@@ -4495,17 +4531,17 @@
       <c r="S34" s="108"/>
       <c r="U34" s="127"/>
       <c r="V34" s="127" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="W34" s="127" t="s">
-        <v>102</v>
-      </c>
-      <c r="X34" s="127" t="s">
         <v>105</v>
       </c>
-      <c r="Y34" s="127"/>
-    </row>
-    <row r="35" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X34" s="165"/>
+      <c r="Y34" s="161"/>
+      <c r="Z34" s="162"/>
+      <c r="AA34" s="161"/>
+    </row>
+    <row r="35" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="128"/>
       <c r="B35" s="125"/>
       <c r="C35" s="63"/>
@@ -4516,11 +4552,11 @@
       <c r="J35" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="K35" s="222">
+      <c r="K35" s="235">
         <f>IF($K$33&gt;0,_xlfn.CEILING.MATH(INDEX(DATA_DRAG_ACCU_EXP, 60)/$K$33),"")</f>
-        <v>107</v>
-      </c>
-      <c r="L35" s="222"/>
+        <v>104</v>
+      </c>
+      <c r="L35" s="235"/>
       <c r="M35" s="127" t="s">
         <v>39</v>
       </c>
@@ -4532,27 +4568,28 @@
       <c r="U35" s="144" t="s">
         <v>96</v>
       </c>
-      <c r="V35" s="145">
-        <v>4</v>
-      </c>
-      <c r="W35" s="150">
+      <c r="V35" s="150">
         <f>VOID_TOTAL_GOLD/VOID_TOTAL_GAMES</f>
-        <v>4.5901639344262293E-2</v>
-      </c>
-      <c r="X35" s="145">
+        <v>5.7220708446866483E-2</v>
+      </c>
+      <c r="W35" s="145">
         <f>VOID_TOTAL_GAMES/VOID_TOTAL_GOLD</f>
-        <v>21.785714285714285</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17.476190476190474</v>
+      </c>
+      <c r="X35" s="161"/>
+      <c r="Y35" s="161"/>
+      <c r="Z35" s="162"/>
+      <c r="AA35" s="161"/>
+    </row>
+    <row r="36" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J36" s="142" t="s">
         <v>87</v>
       </c>
-      <c r="K36" s="222">
+      <c r="K36" s="235">
         <f>IF($K$33&gt;0,_xlfn.CEILING.MATH(INDEX(DATA_DRAG_ACCU_EXP, 80)/$K$33),"")</f>
-        <v>239</v>
-      </c>
-      <c r="L36" s="222"/>
+        <v>234</v>
+      </c>
+      <c r="L36" s="235"/>
       <c r="M36" s="127" t="s">
         <v>39</v>
       </c>
@@ -4561,18 +4598,19 @@
         <v>97</v>
       </c>
       <c r="V36" s="147">
-        <v>264</v>
-      </c>
-      <c r="W36" s="147">
         <f>VOID_TOTAL_SILVER/VOID_TOTAL_GAMES</f>
-        <v>2.1737704918032787</v>
-      </c>
-      <c r="X36" s="151">
+        <v>2.2915531335149866</v>
+      </c>
+      <c r="W36" s="151">
         <f>VOID_TOTAL_GAMES/VOID_TOTAL_SILVER</f>
-        <v>0.46003016591251883</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.43638525564803804</v>
+      </c>
+      <c r="X36" s="161"/>
+      <c r="Y36" s="161"/>
+      <c r="Z36" s="162"/>
+      <c r="AA36" s="161"/>
+    </row>
+    <row r="37" spans="1:27" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="129"/>
       <c r="B37" s="129"/>
       <c r="C37" s="106"/>
@@ -4585,11 +4623,11 @@
       <c r="J37" s="129" t="s">
         <v>88</v>
       </c>
-      <c r="K37" s="223">
+      <c r="K37" s="236">
         <f>IF($K$33&gt;0,_xlfn.CEILING.MATH(INDEX(DATA_DRAG_ACCU_EXP, 100)/$K$33),"")</f>
-        <v>475</v>
-      </c>
-      <c r="L37" s="223"/>
+        <v>464</v>
+      </c>
+      <c r="L37" s="236"/>
       <c r="M37" s="103" t="s">
         <v>39</v>
       </c>
@@ -4601,64 +4639,52 @@
       <c r="T37" s="127" t="s">
         <v>42</v>
       </c>
-      <c r="U37" s="235" t="s">
+      <c r="U37" s="156" t="s">
         <v>106</v>
       </c>
-      <c r="V37" s="236"/>
-      <c r="W37" s="236">
+      <c r="V37" s="157">
         <f>VOID_TOTAL_SILVER2/VOID_TOTAL_SILVER2_GAMES</f>
-        <v>3.1142857142857143</v>
-      </c>
-      <c r="X37" s="237">
+        <v>3.4355828220858897</v>
+      </c>
+      <c r="W37" s="158">
         <f>VOID_TOTAL_SILVER2_GAMES/VOID_TOTAL_SILVER2</f>
-        <v>0.32110091743119268</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+        <v>0.29107142857142859</v>
+      </c>
+      <c r="Z37" s="128"/>
+      <c r="AA37" s="142"/>
+    </row>
+    <row r="38" spans="1:27" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="Q38" s="109"/>
       <c r="S38" s="128"/>
       <c r="T38" s="76">
         <f>VOID_TOTAL_GAMES</f>
-        <v>305</v>
+        <v>367</v>
       </c>
       <c r="U38" s="148" t="s">
         <v>104</v>
       </c>
-      <c r="V38" s="149">
-        <v>18</v>
-      </c>
-      <c r="W38" s="152">
+      <c r="V38" s="152">
         <f>VOID_TOTAL_SPECIAL/VOID_TOTAL_GAMES</f>
-        <v>9.1803278688524587E-2</v>
-      </c>
-      <c r="X38" s="149">
+        <v>8.4468664850136238E-2</v>
+      </c>
+      <c r="W38" s="149">
         <f>VOID_TOTAL_GAMES/VOID_TOTAL_SPECIAL</f>
-        <v>10.892857142857142</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+        <v>11.838709677419354</v>
+      </c>
+      <c r="Z38" s="128"/>
+      <c r="AA38" s="142"/>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="Q39" s="128"/>
       <c r="S39" s="128"/>
       <c r="X39" s="46"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="Q40" s="128"/>
       <c r="S40" s="128"/>
     </row>
   </sheetData>
   <mergeCells count="183">
-    <mergeCell ref="S30:Y32"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="F32:G33"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="K33:M34"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="M30:N31"/>
-    <mergeCell ref="M28:N29"/>
-    <mergeCell ref="M26:N27"/>
     <mergeCell ref="O30:P31"/>
     <mergeCell ref="O28:P29"/>
     <mergeCell ref="O26:P27"/>
@@ -4671,6 +4697,17 @@
     <mergeCell ref="K28:K29"/>
     <mergeCell ref="J28:J29"/>
     <mergeCell ref="K26:K27"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="F32:G33"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="K33:M34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="M30:N31"/>
+    <mergeCell ref="M28:N29"/>
+    <mergeCell ref="M26:N27"/>
     <mergeCell ref="S1:AJ1"/>
     <mergeCell ref="J25:K25"/>
     <mergeCell ref="M25:P25"/>
@@ -4714,6 +4751,7 @@
     <mergeCell ref="AA8:AA9"/>
     <mergeCell ref="AF18:AF19"/>
     <mergeCell ref="AG18:AG19"/>
+    <mergeCell ref="AE18:AE19"/>
     <mergeCell ref="AH6:AH7"/>
     <mergeCell ref="AI4:AI5"/>
     <mergeCell ref="G10:H10"/>
@@ -4782,6 +4820,7 @@
     <mergeCell ref="AB10:AB11"/>
     <mergeCell ref="AB20:AB21"/>
     <mergeCell ref="AC20:AC21"/>
+    <mergeCell ref="AE20:AE21"/>
     <mergeCell ref="AJ24:AJ25"/>
     <mergeCell ref="AI12:AI13"/>
     <mergeCell ref="AJ12:AJ13"/>
@@ -4805,7 +4844,7 @@
     <mergeCell ref="AG24:AG25"/>
     <mergeCell ref="AH24:AH25"/>
     <mergeCell ref="AD18:AD19"/>
-    <mergeCell ref="AE18:AE19"/>
+    <mergeCell ref="S30:W32"/>
     <mergeCell ref="AI24:AI25"/>
     <mergeCell ref="S12:S13"/>
     <mergeCell ref="T12:T13"/>
@@ -4829,7 +4868,6 @@
     <mergeCell ref="AC10:AC11"/>
     <mergeCell ref="AA20:AA21"/>
     <mergeCell ref="AD20:AD21"/>
-    <mergeCell ref="AE20:AE21"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:I3 U27:U29">
     <cfRule type="dataBar" priority="3">
@@ -5067,10 +5105,10 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5087,30 +5125,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="201" t="s">
+      <c r="A1" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="F1" s="201" t="s">
+      <c r="B1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="F1" s="218" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
-      <c r="L1" s="201"/>
-      <c r="N1" s="201" t="s">
+      <c r="G1" s="218"/>
+      <c r="H1" s="218"/>
+      <c r="I1" s="218"/>
+      <c r="J1" s="218"/>
+      <c r="K1" s="218"/>
+      <c r="L1" s="218"/>
+      <c r="N1" s="218" t="s">
         <v>98</v>
       </c>
-      <c r="O1" s="201"/>
-      <c r="P1" s="201"/>
-      <c r="Q1" s="201"/>
-      <c r="R1" s="201"/>
-      <c r="S1" s="201"/>
-      <c r="T1" s="201"/>
+      <c r="O1" s="218"/>
+      <c r="P1" s="218"/>
+      <c r="Q1" s="218"/>
+      <c r="R1" s="218"/>
+      <c r="S1" s="218"/>
+      <c r="T1" s="218"/>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="84"/>
@@ -5167,56 +5205,54 @@
         <v>68</v>
       </c>
       <c r="B3" s="46">
-        <v>277</v>
-      </c>
-      <c r="C3" s="51">
-        <v>15</v>
-      </c>
-      <c r="D3" s="51">
-        <v>167</v>
+        <v>251134</v>
+      </c>
+      <c r="C3" s="166">
+        <v>10</v>
+      </c>
+      <c r="D3" s="166">
+        <v>400</v>
       </c>
       <c r="F3" s="82" t="s">
         <v>68</v>
       </c>
       <c r="G3" s="46">
-        <v>251709</v>
-      </c>
-      <c r="H3" s="154">
-        <v>11</v>
-      </c>
-      <c r="I3" s="154">
-        <v>8186</v>
+        <v>247964</v>
+      </c>
+      <c r="H3" s="167">
+        <v>9</v>
+      </c>
+      <c r="I3" s="167">
+        <v>9603</v>
       </c>
       <c r="J3" s="49">
-        <v>8</v>
+        <v>322</v>
       </c>
       <c r="K3" s="49">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="L3" s="47">
         <f>I3*DRAGEXP_S+J3*DRAGEXP_M+K3*DRAGEXP_L</f>
-        <v>1246400</v>
+        <v>1916450</v>
       </c>
       <c r="N3" s="82" t="s">
         <v>68</v>
       </c>
       <c r="O3" s="46">
-        <v>251709</v>
-      </c>
-      <c r="P3" s="154">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="154">
-        <v>12</v>
-      </c>
-      <c r="R3" s="49">
-        <v>494</v>
-      </c>
-      <c r="S3" s="49">
-        <v>195</v>
-      </c>
-      <c r="T3" s="49">
-        <v>3</v>
+        <v>250339</v>
+      </c>
+      <c r="P3" s="155">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="155">
+        <v>22</v>
+      </c>
+      <c r="R3" s="155">
+        <v>739</v>
+      </c>
+      <c r="S3" s="155"/>
+      <c r="T3" s="155">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5224,56 +5260,54 @@
         <v>69</v>
       </c>
       <c r="B4" s="46">
-        <v>177</v>
-      </c>
-      <c r="C4" s="51">
-        <v>1</v>
-      </c>
-      <c r="D4" s="51">
-        <v>237</v>
+        <v>251134</v>
+      </c>
+      <c r="C4" s="155">
+        <v>0</v>
+      </c>
+      <c r="D4" s="155">
+        <v>418</v>
       </c>
       <c r="F4" s="82" t="s">
         <v>69</v>
       </c>
       <c r="G4" s="46">
-        <v>251709</v>
+        <v>247864</v>
       </c>
       <c r="H4" s="2">
         <v>1</v>
       </c>
       <c r="I4" s="2">
-        <v>8228</v>
+        <v>9734</v>
       </c>
       <c r="J4" s="47">
-        <v>14</v>
+        <v>342</v>
       </c>
       <c r="K4" s="47">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="L4" s="47">
         <f>I4*DRAGEXP_S+J4*DRAGEXP_M+K4*DRAGEXP_L</f>
-        <v>1258700</v>
+        <v>1956100</v>
       </c>
       <c r="N4" s="82" t="s">
         <v>69</v>
       </c>
       <c r="O4" s="46">
-        <v>251609</v>
-      </c>
-      <c r="P4" s="154">
-        <v>-1</v>
-      </c>
-      <c r="Q4" s="154">
-        <v>14</v>
-      </c>
-      <c r="R4" s="49">
-        <v>537</v>
-      </c>
-      <c r="S4" s="49">
-        <v>241</v>
-      </c>
-      <c r="T4" s="49">
-        <v>3</v>
+        <v>250339</v>
+      </c>
+      <c r="P4" s="155">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="155">
+        <v>22</v>
+      </c>
+      <c r="R4" s="155">
+        <v>739</v>
+      </c>
+      <c r="S4" s="155"/>
+      <c r="T4" s="155">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5286,49 +5320,51 @@
       <c r="H5" s="47"/>
       <c r="I5" s="47"/>
       <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
+      <c r="K5" s="49"/>
     </row>
     <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="217" t="s">
+      <c r="B6" s="234" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="217"/>
+      <c r="C6" s="234"/>
       <c r="D6" s="81" t="s">
         <v>15</v>
       </c>
+      <c r="K6" s="167"/>
     </row>
     <row r="7" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>3</v>
       </c>
-      <c r="B7" s="231">
+      <c r="B7" s="244">
         <f>D13</f>
-        <v>6</v>
-      </c>
-      <c r="C7" s="231"/>
+        <v>2</v>
+      </c>
+      <c r="C7" s="244"/>
       <c r="D7" s="68">
         <f>A7*B7</f>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F7" s="78" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="227">
+      <c r="G7" s="240">
         <f>L4-L3</f>
-        <v>12300</v>
-      </c>
-      <c r="H7" s="227"/>
+        <v>39650</v>
+      </c>
+      <c r="H7" s="240"/>
+      <c r="K7" s="167"/>
       <c r="N7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O7" s="222">
+      <c r="O7" s="235">
         <f>(O3-O4)/WINGS_RECOVER_DIAMS*6 + (P3-P4)/WINGS_CONSUME_VOID</f>
-        <v>13</v>
-      </c>
-      <c r="P7" s="222"/>
+        <v>8</v>
+      </c>
+      <c r="P7" s="235"/>
       <c r="R7" s="54"/>
       <c r="S7" s="54"/>
       <c r="T7" s="54"/>
@@ -5337,23 +5373,24 @@
       <c r="A8" s="50">
         <v>4</v>
       </c>
-      <c r="B8" s="232">
+      <c r="B8" s="245">
         <f>D14</f>
-        <v>13</v>
-      </c>
-      <c r="C8" s="232"/>
+        <v>3</v>
+      </c>
+      <c r="C8" s="245"/>
       <c r="D8" s="69">
         <f>A8*B8</f>
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="F8" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="222">
+      <c r="G8" s="235">
         <f>(G3-G4)/WINGS_RECOVER_DIAMS*6 + (H3-H4)/WINGS_CONSUME_DRAGON</f>
-        <v>5</v>
-      </c>
-      <c r="H8" s="222"/>
+        <v>16</v>
+      </c>
+      <c r="H8" s="235"/>
+      <c r="K8" s="167"/>
     </row>
     <row r="9" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="81" t="s">
@@ -5361,15 +5398,16 @@
       </c>
       <c r="B9" s="51">
         <f>SUM(B7:B8)</f>
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C9" s="51">
         <f>SUM(D7:D8)</f>
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="D9" s="81" t="s">
         <v>41</v>
       </c>
+      <c r="K9" s="167"/>
       <c r="N9" s="142"/>
       <c r="O9" s="142" t="s">
         <v>96</v>
@@ -5390,38 +5428,39 @@
       </c>
       <c r="B10" s="51">
         <f>(B3-B4)/WINGS_RECOVER_DIAMS*6 + (C3-C4)/WINGS_CONSUME_IO</f>
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C10" s="51">
         <f>D4-D3</f>
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="D10" s="70">
         <f>IFERROR(C9/B9, "-")</f>
-        <v>3.6842105263157894</v>
+        <v>3.6</v>
       </c>
       <c r="F10" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="230">
+      <c r="G10" s="243">
         <f>IF(G8&gt;0,G7/G8,"")</f>
-        <v>2460</v>
-      </c>
-      <c r="H10" s="230"/>
+        <v>2478.125</v>
+      </c>
+      <c r="H10" s="243"/>
+      <c r="K10" s="167"/>
       <c r="N10" s="142" t="s">
         <v>99</v>
       </c>
       <c r="O10" s="124">
         <f>Q4-Q3</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P10" s="124">
         <f>R4-R3</f>
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="153">
         <f>S4-S3</f>
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="R10" s="124">
         <f>T4-T3</f>
@@ -5429,20 +5468,21 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="167"/>
       <c r="N11" s="142" t="s">
         <v>100</v>
       </c>
       <c r="O11" s="124">
         <f>IFERROR(O10/$O$7,"")</f>
-        <v>0.15384615384615385</v>
+        <v>0</v>
       </c>
       <c r="P11" s="124">
         <f>IFERROR(P10/$O$7,"")</f>
-        <v>3.3076923076923075</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="153">
         <f>IFERROR(Q10/$O$7,"")</f>
-        <v>3.5384615384615383</v>
+        <v>0</v>
       </c>
       <c r="R11" s="124">
         <f>IFERROR(R10/$O$7,"")</f>
@@ -5452,15 +5492,16 @@
       <c r="T11" s="143"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="228" t="s">
+      <c r="A12" s="241" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="228"/>
-      <c r="C12" s="229">
+      <c r="B12" s="241"/>
+      <c r="C12" s="242">
         <f ca="1">NOW()</f>
-        <v>43519.835515162034</v>
-      </c>
-      <c r="D12" s="229"/>
+        <v>43523.987202430559</v>
+      </c>
+      <c r="D12" s="242"/>
+      <c r="K12" s="167"/>
     </row>
     <row r="13" spans="1:20" s="65" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="65">
@@ -5473,11 +5514,11 @@
       </c>
       <c r="C13" s="65">
         <f>Tools!C10</f>
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="D13" s="65">
         <f t="array" ref="D13:D14">MMULT(MINVERSE(Tools!$A$13:$B$14),Tools!$C$13:$C$14)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:20" s="65" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -5489,34 +5530,18 @@
       </c>
       <c r="C14" s="65">
         <f>Tools!B10</f>
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D14" s="65">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N16" s="238">
-        <v>0.83472222222222225</v>
-      </c>
-      <c r="O16" s="2">
-        <v>23</v>
-      </c>
-      <c r="P16" s="2">
-        <v>78</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>15</v>
-      </c>
-      <c r="R16" s="2">
-        <v>554</v>
-      </c>
-      <c r="S16" s="154">
-        <v>268</v>
-      </c>
-      <c r="T16" s="2">
-        <v>5</v>
-      </c>
+      <c r="K16" s="167"/>
+      <c r="N16" s="159"/>
+    </row>
+    <row r="17" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N17" s="159"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -5546,7 +5571,7 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5788,9 +5813,15 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="123" t="str">
+      <c r="A12" s="47">
+        <v>13150</v>
+      </c>
+      <c r="B12" s="47">
+        <v>5</v>
+      </c>
+      <c r="C12" s="123">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2630</v>
       </c>
       <c r="E12" s="48">
         <v>11</v>
@@ -5803,9 +5834,15 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="123" t="str">
+      <c r="A13" s="47">
+        <v>62700</v>
+      </c>
+      <c r="B13" s="47">
+        <v>26</v>
+      </c>
+      <c r="C13" s="123">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2411.5384615384614</v>
       </c>
       <c r="E13" s="48">
         <v>12</v>
@@ -5818,9 +5855,15 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="123" t="str">
+      <c r="A14" s="47">
+        <v>13800</v>
+      </c>
+      <c r="B14" s="47">
+        <v>4</v>
+      </c>
+      <c r="C14" s="123">
         <f t="shared" si="0"/>
-        <v/>
+        <v>3450</v>
       </c>
       <c r="E14" s="48">
         <v>13</v>
@@ -5833,9 +5876,15 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="123" t="str">
+      <c r="A15" s="47">
+        <v>255900</v>
+      </c>
+      <c r="B15" s="47">
+        <v>88</v>
+      </c>
+      <c r="C15" s="123">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2907.9545454545455</v>
       </c>
       <c r="E15" s="48">
         <v>14</v>
@@ -5848,9 +5897,15 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="123" t="str">
+      <c r="A16" s="47">
+        <v>43350</v>
+      </c>
+      <c r="B16" s="47">
+        <v>15</v>
+      </c>
+      <c r="C16" s="123">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2890</v>
       </c>
       <c r="E16" s="48">
         <v>15</v>
@@ -5862,10 +5917,16 @@
         <v>9420</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="123" t="str">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="47">
+        <v>39650</v>
+      </c>
+      <c r="B17" s="47">
+        <v>16</v>
+      </c>
+      <c r="C17" s="123">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2478.125</v>
       </c>
       <c r="E17" s="48">
         <v>16</v>
@@ -5877,7 +5938,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C18" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5892,7 +5953,7 @@
         <v>12300</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C19" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5907,7 +5968,7 @@
         <v>13920</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C20" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5922,7 +5983,7 @@
         <v>15660</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C21" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5937,7 +5998,7 @@
         <v>17520</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C22" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5952,7 +6013,7 @@
         <v>19500</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C23" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5967,7 +6028,7 @@
         <v>21660</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C24" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5982,7 +6043,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5997,7 +6058,7 @@
         <v>26520</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C26" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6012,7 +6073,7 @@
         <v>29220</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C27" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6027,7 +6088,7 @@
         <v>32100</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C28" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6042,7 +6103,7 @@
         <v>35160</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C29" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6057,7 +6118,7 @@
         <v>38400</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C30" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6072,7 +6133,7 @@
         <v>41820</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C31" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6087,7 +6148,7 @@
         <v>45420</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C32" s="123" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7151,13 +7212,14 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9.140625" style="142"/>
-    <col min="4" max="5" width="9.140625" style="154"/>
+    <col min="4" max="4" width="9.140625" style="154"/>
+    <col min="5" max="5" width="0" style="154" hidden="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="142"/>
   </cols>
   <sheetData>
@@ -7407,27 +7469,96 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="142">
+        <v>30</v>
+      </c>
+      <c r="B12" s="142">
+        <v>1</v>
+      </c>
+      <c r="C12" s="142">
+        <v>87</v>
+      </c>
+      <c r="D12" s="154">
+        <v>114</v>
+      </c>
       <c r="E12" s="154">
         <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="F12" s="142">
+        <v>1</v>
+      </c>
+      <c r="G12" s="155" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="142">
+        <v>4</v>
+      </c>
+      <c r="B13" s="142">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="142">
+        <v>5</v>
+      </c>
       <c r="E13" s="154">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F13" s="142">
+        <v>0</v>
+      </c>
+      <c r="G13" s="155" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="142">
+        <v>17</v>
+      </c>
+      <c r="B14" s="142">
+        <v>3</v>
+      </c>
+      <c r="C14" s="142">
+        <v>54</v>
+      </c>
+      <c r="D14" s="154">
+        <v>68</v>
+      </c>
       <c r="E14" s="154">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="F14" s="142">
+        <v>2</v>
+      </c>
+      <c r="G14" s="155" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="142">
+        <v>11</v>
+      </c>
+      <c r="B15" s="142">
+        <v>3</v>
+      </c>
+      <c r="C15" s="142">
+        <v>32</v>
+      </c>
+      <c r="D15" s="154">
+        <v>51</v>
+      </c>
       <c r="E15" s="154">
         <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F15" s="142">
         <v>0</v>
+      </c>
+      <c r="G15" s="155" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -7520,8 +7651,8 @@
   </sheetPr>
   <dimension ref="A1:X32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7542,33 +7673,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="246" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="233"/>
-      <c r="C1" s="233"/>
-      <c r="D1" s="233"/>
-      <c r="E1" s="233"/>
-      <c r="F1" s="233"/>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="233"/>
-      <c r="J1" s="233"/>
-      <c r="K1" s="233"/>
-      <c r="L1" s="233"/>
-      <c r="M1" s="233"/>
-      <c r="N1" s="233"/>
-      <c r="O1" s="233"/>
-      <c r="Q1" s="234" t="s">
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
+      <c r="H1" s="246"/>
+      <c r="I1" s="246"/>
+      <c r="J1" s="246"/>
+      <c r="K1" s="246"/>
+      <c r="L1" s="246"/>
+      <c r="M1" s="246"/>
+      <c r="N1" s="246"/>
+      <c r="O1" s="246"/>
+      <c r="Q1" s="247" t="s">
         <v>90</v>
       </c>
-      <c r="R1" s="234"/>
-      <c r="S1" s="234"/>
-      <c r="T1" s="234"/>
-      <c r="U1" s="234"/>
-      <c r="V1" s="234"/>
-      <c r="W1" s="234"/>
-      <c r="X1" s="234"/>
+      <c r="R1" s="247"/>
+      <c r="S1" s="247"/>
+      <c r="T1" s="247"/>
+      <c r="U1" s="247"/>
+      <c r="V1" s="247"/>
+      <c r="W1" s="247"/>
+      <c r="X1" s="247"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
@@ -7964,9 +8095,15 @@
         <f t="shared" si="2"/>
         <v>3.6842105263157894</v>
       </c>
-      <c r="L7" s="120" t="str">
+      <c r="J7" s="20">
+        <v>2</v>
+      </c>
+      <c r="K7" s="20">
+        <v>9</v>
+      </c>
+      <c r="L7" s="120">
         <f t="shared" si="3"/>
-        <v/>
+        <v>3.8181818181818183</v>
       </c>
       <c r="O7" s="122" t="str">
         <f t="shared" si="4"/>
@@ -8012,13 +8149,25 @@
         <f t="shared" si="1"/>
         <v>3.4133333333333336</v>
       </c>
-      <c r="I8" s="118" t="str">
+      <c r="G8" s="19">
+        <v>0</v>
+      </c>
+      <c r="H8" s="19">
+        <v>1</v>
+      </c>
+      <c r="I8" s="118">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L8" s="120" t="str">
+        <v>4</v>
+      </c>
+      <c r="J8" s="20">
+        <v>2</v>
+      </c>
+      <c r="K8" s="20">
+        <v>4</v>
+      </c>
+      <c r="L8" s="120">
         <f t="shared" si="3"/>
-        <v/>
+        <v>3.6666666666666665</v>
       </c>
       <c r="O8" s="122" t="str">
         <f t="shared" si="4"/>
@@ -8418,9 +8567,15 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F16" s="116" t="str">
+      <c r="D16" s="17">
+        <v>5</v>
+      </c>
+      <c r="E16" s="17">
+        <v>0</v>
+      </c>
+      <c r="F16" s="116">
         <f t="shared" si="1"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="I16" s="118" t="str">
         <f t="shared" si="2"/>
@@ -8464,9 +8619,15 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F17" s="116" t="str">
+      <c r="D17" s="17">
+        <v>19</v>
+      </c>
+      <c r="E17" s="17">
+        <v>13</v>
+      </c>
+      <c r="F17" s="116">
         <f t="shared" si="1"/>
-        <v/>
+        <v>3.40625</v>
       </c>
       <c r="I17" s="118" t="str">
         <f t="shared" si="2"/>
@@ -9295,10 +9456,10 @@
   <sheetPr codeName="Sheet7">
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16:Y16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9306,7 +9467,7 @@
     <col min="1" max="16384" width="2.85546875" style="75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="75">
         <v>2</v>
       </c>
@@ -9328,8 +9489,11 @@
       <c r="G1" s="75">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="75">
         <v>3</v>
       </c>
@@ -9351,8 +9515,11 @@
       <c r="G2" s="75">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="75">
         <v>2</v>
       </c>
@@ -9374,8 +9541,11 @@
       <c r="G3" s="75">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="75">
         <v>2</v>
       </c>
@@ -9397,8 +9567,11 @@
       <c r="G4" s="75">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="75">
         <v>2</v>
       </c>
@@ -9420,8 +9593,11 @@
       <c r="G5" s="75">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="75">
         <v>3</v>
       </c>
@@ -9443,8 +9619,11 @@
       <c r="G6" s="75">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="75">
         <v>2</v>
       </c>
@@ -9466,8 +9645,11 @@
       <c r="G7" s="75">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="75">
         <v>2</v>
       </c>
@@ -9489,8 +9671,11 @@
       <c r="G8" s="75">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="75">
         <v>2</v>
       </c>
@@ -9512,8 +9697,11 @@
       <c r="G9" s="75">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="75">
         <v>2</v>
       </c>
@@ -9535,8 +9723,11 @@
       <c r="G10" s="75">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="75">
         <v>2</v>
       </c>
@@ -9558,8 +9749,11 @@
       <c r="G11" s="75">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="75">
         <v>2</v>
       </c>
@@ -9581,8 +9775,11 @@
       <c r="G12" s="75">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="75">
         <v>2</v>
       </c>
@@ -9604,8 +9801,11 @@
       <c r="G13" s="75">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="75">
         <v>2</v>
       </c>
@@ -9624,8 +9824,11 @@
       <c r="F14" s="75">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="75">
         <v>2</v>
       </c>
@@ -9644,8 +9847,11 @@
       <c r="F15" s="75">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="75">
         <v>2</v>
       </c>
@@ -9664,8 +9870,11 @@
       <c r="F16" s="75">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="75">
         <v>2</v>
       </c>
@@ -9684,8 +9893,11 @@
       <c r="F17" s="75">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="75">
         <v>2</v>
       </c>
@@ -9704,8 +9916,11 @@
       <c r="F18" s="75">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="75">
         <v>2</v>
       </c>
@@ -9724,8 +9939,11 @@
       <c r="F19" s="75">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="75">
         <v>2</v>
       </c>
@@ -9742,6 +9960,9 @@
         <v>2</v>
       </c>
       <c r="F20" s="75">
+        <v>2</v>
+      </c>
+      <c r="G20" s="75">
         <v>2</v>
       </c>
     </row>

</xml_diff>